<commit_message>
improving excell with OMP_THREADS=10
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="600" windowWidth="34140" windowHeight="19940" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="3120" yWindow="940" windowWidth="34140" windowHeight="19940" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_timings.txt" sheetId="1" r:id="rId1"/>
     <sheet name="Graphs OMP_NUM_THREADS=20" sheetId="2" r:id="rId2"/>
-    <sheet name="Thread Mappings" sheetId="3" r:id="rId3"/>
+    <sheet name="Graphs OMP_NUM_THREADS=10" sheetId="4" r:id="rId3"/>
+    <sheet name="Thread Mappings" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="thread_mapping_experiments" localSheetId="2">'Thread Mappings'!$A$1:$B$5205</definedName>
+    <definedName name="thread_mapping_experiments" localSheetId="3">'Thread Mappings'!$A$1:$B$5205</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10565" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10617" uniqueCount="370">
   <si>
     <t>----------------------</t>
   </si>
@@ -1119,6 +1120,9 @@
     <t>(master, threads) = All threads execute in CPUID=0</t>
   </si>
   <si>
+    <t>Notes:</t>
+  </si>
+  <si>
     <t>(master, cores) = All threads execute in the same core as the master. In this case the first core which contains CPUID=0-7. Threads are distributed to 8 CPUIDs</t>
   </si>
   <si>
@@ -1141,6 +1145,9 @@
   </si>
   <si>
     <t>(false, *) threads can migrate and are not binded to a specific thread, core or socket. This migration makes it less impactful on data placement, but suffers from performance.</t>
+  </si>
+  <si>
+    <t>(true, threads) seems to be equivalent to (close,threads) according to the thread mappings</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1203,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="93">
+  <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1297,7 +1334,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="93">
+  <cellStyles count="123">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1344,6 +1381,21 @@
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1390,6 +1442,21 @@
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2194,7 +2261,7 @@
             <c:numRef>
               <c:f>'Graphs OMP_NUM_THREADS=20'!$B$90:$B$104</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>8.99248098299722</c:v>
@@ -2320,7 +2387,7 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2346,20 +2413,987 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+              <a:lnSpc>
+                <a:spcPct val="100000"/>
+              </a:lnSpc>
+              <a:spcBef>
+                <a:spcPts val="0"/>
+              </a:spcBef>
+              <a:spcAft>
+                <a:spcPts val="0"/>
+              </a:spcAft>
+              <a:buClrTx/>
+              <a:buSzTx/>
+              <a:buFontTx/>
+              <a:buNone/>
+              <a:tabLst/>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time for Affine and Non Affine Accesses</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Affine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$J$2:$J$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$2:$K$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>15.967569817003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.3149772839969</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.8796826359757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.74924854998243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.9599736139934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.92893046300741</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.32121792400721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.97052923101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.33048951800446</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.01099709700793</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.03875824500573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.12055050898925</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.98585961700882</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.95102254601079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.11385154200252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Non-affine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$J$2:$J$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$L$2:$L$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>15.9634523389977</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.2745326239964</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.7783720720035</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.68555049001588</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.9650519969873</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.45411046300432</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.94314495899016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.54107747599482</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.97303582201129</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.73803968401625</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.80434663599589</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.97387528698891</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.8228360240173</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.85941002299659</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.60011122998548</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2035570424"/>
+        <c:axId val="-2052007512"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2035570424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OpenMP Affinity</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2052007512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2052007512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> (Seconds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2035570424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Improvement of Affine vs. Non-Affine Accesses</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Improvement %</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$J$38:$J$52</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$38:$K$52</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.000318194949235261</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17930777347908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.187258725327052</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.192069560881187</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.192928487098745</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.241462400522004</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.251941197444194</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.273453281894179</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.280313381861853</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.307821259520285</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.477305892055196</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2051231192"/>
+        <c:axId val="-2036030888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2051231192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2036030888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2036030888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Improvement (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2051231192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Performance with Affine Accesses</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$71</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Affine</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$J$72:$J$86</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Graphs OMP_NUM_THREADS=10'!$K$72:$K$86</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>15.967569817003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28.3149772839969</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19.8796826359757</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.74924854998243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.9599736139934</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.92893046300741</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.32121792400721</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.97052923101</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.33048951800446</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.01099709700793</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.03875824500573</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.12055050898925</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.98585961700882</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.95102254601079</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.11385154200252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2045126280"/>
+        <c:axId val="-2045971160"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2045126280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2045971160"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2045971160"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Time (Seconds)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2045126280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2424,6 +3458,101 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="13" name="Chart 12"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>641350</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2286000</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>69850</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2070100</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>107950</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>2362200</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2769,8 +3898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H720"/>
   <sheetViews>
-    <sheetView topLeftCell="A335" workbookViewId="0">
-      <selection activeCell="N343" sqref="N343"/>
+    <sheetView topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="A121" sqref="A121:B240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -7248,14 +8377,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E104"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="72.5" customWidth="1"/>
     <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -7536,7 +8666,7 @@
         <v>1.7828911239283866E-3</v>
       </c>
       <c r="E56" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -7558,7 +8688,7 @@
         <v>0.41455599694980522</v>
       </c>
       <c r="E58" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -7569,7 +8699,7 @@
         <v>0.4671148487428996</v>
       </c>
       <c r="E59" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -7580,7 +8710,7 @@
         <v>0.58262659045645404</v>
       </c>
       <c r="E60" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -7591,7 +8721,7 @@
         <v>0.60125267953439354</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -7610,7 +8740,7 @@
         <v>0.61863525724807433</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -7621,18 +8751,21 @@
         <v>0.63514208985572995</v>
       </c>
       <c r="E64" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>32</v>
       </c>
       <c r="B65" s="1">
         <v>0.65541422208192057</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="E65" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -7640,9 +8773,14 @@
         <v>0.70749910817936301</v>
       </c>
     </row>
+    <row r="83" spans="1:5">
+      <c r="E83" t="s">
+        <v>360</v>
+      </c>
+    </row>
     <row r="84" spans="1:5">
       <c r="E84" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -7835,10 +8973,509 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="J1:M86"/>
+  <sheetViews>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="10" max="10" width="36.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="10:13">
+      <c r="K1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="10:13">
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2">
+        <v>15.967569817003</v>
+      </c>
+      <c r="L2">
+        <v>15.963452338997699</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="10:13">
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <v>28.3149772839969</v>
+      </c>
+      <c r="L3">
+        <v>28.2745326239964</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="10:13">
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4">
+        <v>19.879682635975701</v>
+      </c>
+      <c r="L4">
+        <v>19.778372072003499</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="10:13">
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5">
+        <v>6.74924854998243</v>
+      </c>
+      <c r="L5">
+        <v>6.6855504900158804</v>
+      </c>
+      <c r="M5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="10:13">
+      <c r="J6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K6">
+        <v>15.9599736139934</v>
+      </c>
+      <c r="L6">
+        <v>15.965051996987301</v>
+      </c>
+      <c r="M6" s="1">
+        <v>3.1819494923526081E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="10:13">
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7">
+        <v>2.92893046300741</v>
+      </c>
+      <c r="L7">
+        <v>3.4541104630043198</v>
+      </c>
+      <c r="M7" s="1">
+        <v>0.17930777347908008</v>
+      </c>
+    </row>
+    <row r="8" spans="10:13">
+      <c r="J8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8">
+        <v>3.3212179240072102</v>
+      </c>
+      <c r="L8">
+        <v>3.9431449589901599</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0.18725872532705251</v>
+      </c>
+    </row>
+    <row r="9" spans="10:13">
+      <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9">
+        <v>2.97052923101</v>
+      </c>
+      <c r="L9">
+        <v>3.54107747599482</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0.19206956088118673</v>
+      </c>
+    </row>
+    <row r="10" spans="10:13">
+      <c r="J10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10">
+        <v>3.3304895180044598</v>
+      </c>
+      <c r="L10">
+        <v>3.97303582201129</v>
+      </c>
+      <c r="M10" s="1">
+        <v>0.19292848709874541</v>
+      </c>
+    </row>
+    <row r="11" spans="10:13">
+      <c r="J11" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11">
+        <v>3.0109970970079298</v>
+      </c>
+      <c r="L11">
+        <v>3.73803968401625</v>
+      </c>
+      <c r="M11" s="1">
+        <v>0.24146240052200402</v>
+      </c>
+    </row>
+    <row r="12" spans="10:13">
+      <c r="J12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12">
+        <v>3.03875824500573</v>
+      </c>
+      <c r="L12">
+        <v>3.80434663599589</v>
+      </c>
+      <c r="M12" s="1">
+        <v>0.25194119744419363</v>
+      </c>
+    </row>
+    <row r="13" spans="10:13">
+      <c r="J13" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13">
+        <v>3.12055050898925</v>
+      </c>
+      <c r="L13">
+        <v>3.97387528698891</v>
+      </c>
+      <c r="M13" s="1">
+        <v>0.27345328189417861</v>
+      </c>
+    </row>
+    <row r="14" spans="10:13">
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14">
+        <v>2.9858596170088201</v>
+      </c>
+      <c r="L14">
+        <v>3.8228360240172998</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0.28031338186185306</v>
+      </c>
+    </row>
+    <row r="15" spans="10:13">
+      <c r="J15" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15">
+        <v>2.9510225460107899</v>
+      </c>
+      <c r="L15">
+        <v>3.85941002299659</v>
+      </c>
+      <c r="M15" s="1">
+        <v>0.30782125952028516</v>
+      </c>
+    </row>
+    <row r="16" spans="10:13">
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16">
+        <v>3.1138515420025201</v>
+      </c>
+      <c r="L16">
+        <v>4.6001112299854796</v>
+      </c>
+      <c r="M16" s="1">
+        <v>0.47730589205519569</v>
+      </c>
+    </row>
+    <row r="37" spans="10:11">
+      <c r="K37" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="10:11">
+      <c r="J38" t="s">
+        <v>36</v>
+      </c>
+      <c r="K38" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="10:11">
+      <c r="J39" t="s">
+        <v>24</v>
+      </c>
+      <c r="K39" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="10:11">
+      <c r="J40" t="s">
+        <v>29</v>
+      </c>
+      <c r="K40" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="10:11">
+      <c r="J41" t="s">
+        <v>34</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="10:11">
+      <c r="J42" t="s">
+        <v>22</v>
+      </c>
+      <c r="K42" s="1">
+        <v>3.1819494923526081E-4</v>
+      </c>
+    </row>
+    <row r="43" spans="10:11">
+      <c r="J43" t="s">
+        <v>23</v>
+      </c>
+      <c r="K43" s="1">
+        <v>0.17930777347908008</v>
+      </c>
+    </row>
+    <row r="44" spans="10:11">
+      <c r="J44" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="1">
+        <v>0.18725872532705251</v>
+      </c>
+    </row>
+    <row r="45" spans="10:11">
+      <c r="J45" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="1">
+        <v>0.19206956088118673</v>
+      </c>
+    </row>
+    <row r="46" spans="10:11">
+      <c r="J46" t="s">
+        <v>26</v>
+      </c>
+      <c r="K46" s="1">
+        <v>0.19292848709874541</v>
+      </c>
+    </row>
+    <row r="47" spans="10:11">
+      <c r="J47" t="s">
+        <v>25</v>
+      </c>
+      <c r="K47" s="1">
+        <v>0.24146240052200402</v>
+      </c>
+    </row>
+    <row r="48" spans="10:11">
+      <c r="J48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K48" s="1">
+        <v>0.25194119744419363</v>
+      </c>
+    </row>
+    <row r="49" spans="10:11">
+      <c r="J49" t="s">
+        <v>30</v>
+      </c>
+      <c r="K49" s="1">
+        <v>0.27345328189417861</v>
+      </c>
+    </row>
+    <row r="50" spans="10:11">
+      <c r="J50" t="s">
+        <v>33</v>
+      </c>
+      <c r="K50" s="1">
+        <v>0.28031338186185306</v>
+      </c>
+    </row>
+    <row r="51" spans="10:11">
+      <c r="J51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K51" s="1">
+        <v>0.30782125952028516</v>
+      </c>
+    </row>
+    <row r="52" spans="10:11">
+      <c r="J52" t="s">
+        <v>37</v>
+      </c>
+      <c r="K52" s="1">
+        <v>0.47730589205519569</v>
+      </c>
+    </row>
+    <row r="71" spans="10:11">
+      <c r="K71" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="10:11">
+      <c r="J72" t="s">
+        <v>36</v>
+      </c>
+      <c r="K72">
+        <v>15.967569817003</v>
+      </c>
+    </row>
+    <row r="73" spans="10:11">
+      <c r="J73" t="s">
+        <v>24</v>
+      </c>
+      <c r="K73">
+        <v>28.3149772839969</v>
+      </c>
+    </row>
+    <row r="74" spans="10:11">
+      <c r="J74" t="s">
+        <v>29</v>
+      </c>
+      <c r="K74">
+        <v>19.879682635975701</v>
+      </c>
+    </row>
+    <row r="75" spans="10:11">
+      <c r="J75" t="s">
+        <v>34</v>
+      </c>
+      <c r="K75">
+        <v>6.74924854998243</v>
+      </c>
+    </row>
+    <row r="76" spans="10:11">
+      <c r="J76" t="s">
+        <v>22</v>
+      </c>
+      <c r="K76">
+        <v>15.9599736139934</v>
+      </c>
+    </row>
+    <row r="77" spans="10:11">
+      <c r="J77" t="s">
+        <v>23</v>
+      </c>
+      <c r="K77">
+        <v>2.92893046300741</v>
+      </c>
+    </row>
+    <row r="78" spans="10:11">
+      <c r="J78" t="s">
+        <v>27</v>
+      </c>
+      <c r="K78">
+        <v>3.3212179240072102</v>
+      </c>
+    </row>
+    <row r="79" spans="10:11">
+      <c r="J79" t="s">
+        <v>28</v>
+      </c>
+      <c r="K79">
+        <v>2.97052923101</v>
+      </c>
+    </row>
+    <row r="80" spans="10:11">
+      <c r="J80" t="s">
+        <v>26</v>
+      </c>
+      <c r="K80">
+        <v>3.3304895180044598</v>
+      </c>
+    </row>
+    <row r="81" spans="10:11">
+      <c r="J81" t="s">
+        <v>25</v>
+      </c>
+      <c r="K81">
+        <v>3.0109970970079298</v>
+      </c>
+    </row>
+    <row r="82" spans="10:11">
+      <c r="J82" t="s">
+        <v>31</v>
+      </c>
+      <c r="K82">
+        <v>3.03875824500573</v>
+      </c>
+    </row>
+    <row r="83" spans="10:11">
+      <c r="J83" t="s">
+        <v>30</v>
+      </c>
+      <c r="K83">
+        <v>3.12055050898925</v>
+      </c>
+    </row>
+    <row r="84" spans="10:11">
+      <c r="J84" t="s">
+        <v>33</v>
+      </c>
+      <c r="K84">
+        <v>2.9858596170088201</v>
+      </c>
+    </row>
+    <row r="85" spans="10:11">
+      <c r="J85" t="s">
+        <v>32</v>
+      </c>
+      <c r="K85">
+        <v>2.9510225460107899</v>
+      </c>
+    </row>
+    <row r="86" spans="10:11">
+      <c r="J86" t="s">
+        <v>37</v>
+      </c>
+      <c r="K86">
+        <v>3.1138515420025201</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="J2:M16">
+    <sortCondition ref="M2:M16"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5204"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
-      <selection activeCell="G707" sqref="G707"/>
+    <sheetView topLeftCell="A281" workbookViewId="0">
+      <selection activeCell="A374" sqref="A374"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
Adding HW Analysis for 20 threads.
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="120" windowWidth="29000" windowHeight="14340" tabRatio="644" activeTab="4"/>
+    <workbookView xWindow="40" yWindow="20" windowWidth="27320" windowHeight="14340" tabRatio="798" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_timings.txt" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Graphs OMP_NUM_THREADS=10" sheetId="4" r:id="rId3"/>
     <sheet name="Thread Mappings" sheetId="3" r:id="rId4"/>
     <sheet name="Comparing 10 and 20 THREADS" sheetId="5" r:id="rId5"/>
+    <sheet name="HW 20 Analysis" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="thread_mapping_experiments" localSheetId="3">'Thread Mappings'!$A$1:$B$5205</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10692" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10720" uniqueCount="387">
   <si>
     <t>----------------------</t>
   </si>
@@ -1171,6 +1172,36 @@
   <si>
     <t>Notes for improvements:</t>
   </si>
+  <si>
+    <t>PM_CMPLU_STALL_DCACHE_MISS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_L2L3</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_L2L3_CONFLICT</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_L2L3_NO_CONFLICT</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_L3MISS</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_LMEM</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_L21_L31</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_REMOTE</t>
+  </si>
+  <si>
+    <t>\_PM_CMPLU_STALL_DMISS_DISTANT</t>
+  </si>
 </sst>
 </file>
 
@@ -1235,7 +1266,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="219">
+  <cellStyleXfs count="235">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1455,8 +1486,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1465,8 +1512,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="219">
+  <cellStyles count="235">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1576,6 +1632,14 @@
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1685,6 +1749,14 @@
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2095,403 +2167,6 @@
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10 Threads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>(true, threads)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(close, threads)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(master, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(master, cores)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(master, threads)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(spread, threads)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(false, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(false, cores)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(false, threads)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(true, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>(spread, cores)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>(close, cores)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>(true, cores)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>(close, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>(spread, sockets)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$B$2:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.000318194949235261</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.17930777347908</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.273453281894179</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.241462400522004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.477305892055196</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.251941197444194</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.192069560881187</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.187258725327052</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.192928487098745</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.307821259520285</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.280313381861853</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20 Threads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>(true, threads)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(close, threads)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(master, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(master, cores)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(master, threads)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(spread, threads)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(false, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(false, cores)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(false, threads)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(true, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>(spread, cores)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>(close, cores)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>(true, cores)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>(close, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>(spread, sockets)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$C$2:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000728873528646939</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.00178289112392839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.377096545185983</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.414555996949805</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.4671148487429</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.582626590456454</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.601252679534393</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.60479320761319</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.618635257248074</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.63514208985573</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65541422208192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.707499108179363</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2095269464"/>
-        <c:axId val="2096070808"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2095269464"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="1" i="0" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2096070808"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2096070808"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Improvement (%)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095269464"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -3983,432 +3658,6 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>20 Threads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>(true, threads)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(close, threads)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(master, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(master, cores)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(master, threads)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(spread, threads)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(false, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(false, cores)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(false, threads)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(true, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>(spread, cores)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>(close, cores)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>(true, cores)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>(close, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>(spread, sockets)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$C$2:$C$16</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.000728873528646939</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.00178289112392839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.377096545185983</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.414555996949805</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.4671148487429</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.582626590456454</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.601252679534393</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.60479320761319</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.618635257248074</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.63514208985573</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.65541422208192</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.707499108179363</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>10 Threads</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>(true, threads)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(close, threads)</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>(master, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>(master, cores)</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>(master, threads)</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>(spread, threads)</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>(false, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>(false, cores)</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>(false, threads)</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>(true, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>(spread, cores)</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>(close, cores)</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>(true, cores)</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>(close, sockets)</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>(spread, sockets)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Comparing 10 and 20 THREADS'!$B$2:$B$16</c:f>
-              <c:numCache>
-                <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.000318194949235261</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.17930777347908</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.273453281894179</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.241462400522004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.477305892055196</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.251941197444194</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.192069560881187</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.187258725327052</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.192928487098745</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.307821259520285</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.280313381861853</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="2080438888"/>
-        <c:axId val="2080440632"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2080438888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="1" i="0" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080440632"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2080440632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
-                  <a:lnSpc>
-                    <a:spcPct val="100000"/>
-                  </a:lnSpc>
-                  <a:spcBef>
-                    <a:spcPts val="0"/>
-                  </a:spcBef>
-                  <a:spcAft>
-                    <a:spcPts val="0"/>
-                  </a:spcAft>
-                  <a:buClrTx/>
-                  <a:buSzTx/>
-                  <a:buFontTx/>
-                  <a:buNone/>
-                  <a:tabLst/>
-                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:sysClr val="windowText" lastClr="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1000" b="1" i="0" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:effectLst/>
-                  </a:rPr>
-                  <a:t>Improvement (%)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US">
-                  <a:effectLst/>
-                </a:endParaRPr>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="0%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080438888"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
               <c:f>'Comparing 10 and 20 THREADS'!$B$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -4751,7 +4000,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -5103,6 +4352,403 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>10 Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.000318194949235261</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17930777347908</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.273453281894179</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.241462400522004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.477305892055196</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.251941197444194</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.192069560881187</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.187258725327052</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.192928487098745</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.307821259520285</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.280313381861853</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>20 Threads</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$A$2:$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(true, threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(close, threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(master, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(master, cores)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master, threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(false, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(false, cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(false, threads)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(true, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(close, cores)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(true, cores)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(close, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Comparing 10 and 20 THREADS'!$C$2:$C$16</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.000728873528646939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00178289112392839</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.377096545185983</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.414555996949805</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.4671148487429</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.582626590456454</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.601252679534393</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.60479320761319</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.618635257248074</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.63514208985573</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.65541422208192</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.707499108179363</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2095269464"/>
+        <c:axId val="2096070808"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2095269464"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2096070808"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2096070808"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Improvement (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2095269464"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -5297,36 +4943,6 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>101600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>558800</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>203200</xdr:colOff>
       <xdr:row>24</xdr:row>
@@ -5349,7 +4965,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5379,7 +4995,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5409,7 +5025,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10823,8 +10439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="J1:M86"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L16"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -50916,8 +50532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -51139,10 +50755,10 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
@@ -51321,10 +50937,10 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C44" s="5"/>
+      <c r="C44" s="6"/>
       <c r="N44" t="s">
         <v>367</v>
       </c>
@@ -51540,4 +51156,173 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="48.1640625" customWidth="1"/>
+    <col min="2" max="2" width="26" style="5" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="6" width="24.5" customWidth="1"/>
+    <col min="7" max="7" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>377</v>
+      </c>
+      <c r="B4" s="5">
+        <v>98550789721</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>379</v>
+      </c>
+      <c r="B5" s="5">
+        <v>80824433794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>380</v>
+      </c>
+      <c r="B6" s="5">
+        <v>44859484877</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>381</v>
+      </c>
+      <c r="B7" s="7">
+        <v>35964948917</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>382</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1695754759</v>
+      </c>
+      <c r="C8" t="s">
+        <v>378</v>
+      </c>
+      <c r="D8" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>383</v>
+      </c>
+      <c r="B9" s="5">
+        <v>493965751</v>
+      </c>
+      <c r="C9" t="s">
+        <v>378</v>
+      </c>
+      <c r="D9" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>384</v>
+      </c>
+      <c r="B10" s="5">
+        <v>446101625</v>
+      </c>
+      <c r="C10" t="s">
+        <v>378</v>
+      </c>
+      <c r="D10" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>385</v>
+      </c>
+      <c r="B11" s="5">
+        <v>325890614</v>
+      </c>
+      <c r="C11" t="s">
+        <v>378</v>
+      </c>
+      <c r="D11" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>386</v>
+      </c>
+      <c r="B12" s="7">
+        <v>429796769</v>
+      </c>
+      <c r="C12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D12" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="C13" t="s">
+        <v>378</v>
+      </c>
+      <c r="D13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="C14" t="s">
+        <v>378</v>
+      </c>
+      <c r="D14" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="C15" t="s">
+        <v>378</v>
+      </c>
+      <c r="D15" t="s">
+        <v>378</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
improvement hw counters excel
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="20" windowWidth="27320" windowHeight="14340" tabRatio="798" activeTab="6"/>
+    <workbookView xWindow="40" yWindow="20" windowWidth="32100" windowHeight="18040" tabRatio="798" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_timings.txt" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11554" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11555" uniqueCount="407">
   <si>
     <t>----------------------</t>
   </si>
@@ -1260,18 +1260,27 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Improvement</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1324,333 +1333,347 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="313">
+  <cellStyleXfs count="326">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="313" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="313">
+  <cellStyles count="326">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1807,6 +1830,12 @@
     <cellStyle name="Followed Hyperlink" xfId="308" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="310" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="315" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="317" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="319" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1963,7 +1992,14 @@
     <cellStyle name="Hyperlink" xfId="307" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="309" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="314" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="316" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="318" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="313" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2013,7 +2049,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2278,11 +2313,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080105416"/>
-        <c:axId val="2080110904"/>
+        <c:axId val="-2128053976"/>
+        <c:axId val="-2128047048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080105416"/>
+        <c:axId val="-2128053976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2317,7 +2352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080110904"/>
+        <c:crossAx val="-2128047048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2325,7 +2360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080110904"/>
+        <c:axId val="-2128047048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2348,21 +2383,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080105416"/>
+        <c:crossAx val="-2128053976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2412,7 +2445,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2563,11 +2595,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080226376"/>
-        <c:axId val="2079696712"/>
+        <c:axId val="-2127974616"/>
+        <c:axId val="-2127969048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080226376"/>
+        <c:axId val="-2127974616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2589,13 +2621,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079696712"/>
+        <c:crossAx val="-2127969048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2603,7 +2634,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079696712"/>
+        <c:axId val="-2127969048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2631,14 +2662,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080226376"/>
+        <c:crossAx val="-2127974616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2685,7 +2715,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2827,11 +2856,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2079726472"/>
-        <c:axId val="2079678440"/>
+        <c:axId val="-2127939784"/>
+        <c:axId val="-2127934296"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079726472"/>
+        <c:axId val="-2127939784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2853,13 +2882,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079678440"/>
+        <c:crossAx val="-2127934296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2867,7 +2895,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079678440"/>
+        <c:axId val="-2127934296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,21 +2918,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079726472"/>
+        <c:crossAx val="-2127939784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3195,11 +3221,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2079613240"/>
-        <c:axId val="2079618920"/>
+        <c:axId val="-2127887928"/>
+        <c:axId val="-2127882232"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079613240"/>
+        <c:axId val="-2127887928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3225,13 +3251,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079618920"/>
+        <c:crossAx val="-2127882232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3239,7 +3264,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079618920"/>
+        <c:axId val="-2127882232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3267,21 +3292,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079613240"/>
+        <c:crossAx val="-2127887928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3331,7 +3354,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3482,11 +3504,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2080146776"/>
-        <c:axId val="2080221976"/>
+        <c:axId val="-2127851192"/>
+        <c:axId val="-2127845624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2080146776"/>
+        <c:axId val="-2127851192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3508,13 +3530,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080221976"/>
+        <c:crossAx val="-2127845624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3522,7 +3543,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2080221976"/>
+        <c:axId val="-2127845624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3545,14 +3566,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2080146776"/>
+        <c:crossAx val="-2127851192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3604,7 +3624,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3746,11 +3765,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2079806968"/>
-        <c:axId val="2079812472"/>
+        <c:axId val="-2127816168"/>
+        <c:axId val="-2127810664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2079806968"/>
+        <c:axId val="-2127816168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3772,13 +3791,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079812472"/>
+        <c:crossAx val="-2127810664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3786,7 +3804,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2079812472"/>
+        <c:axId val="-2127810664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3809,21 +3827,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2079806968"/>
+        <c:crossAx val="-2127816168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4114,11 +4130,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2085574872"/>
-        <c:axId val="2090367320"/>
+        <c:axId val="-2129619928"/>
+        <c:axId val="-2129625496"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2085574872"/>
+        <c:axId val="-2129619928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4140,13 +4156,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2090367320"/>
+        <c:crossAx val="-2129625496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4154,7 +4169,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2090367320"/>
+        <c:axId val="-2129625496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4177,21 +4192,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2085574872"/>
+        <c:crossAx val="-2129619928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4466,11 +4479,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2078408040"/>
-        <c:axId val="2122438168"/>
+        <c:axId val="-2129657800"/>
+        <c:axId val="-2126236328"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2078408040"/>
+        <c:axId val="-2129657800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4492,13 +4505,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2122438168"/>
+        <c:crossAx val="-2126236328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4506,7 +4518,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2122438168"/>
+        <c:axId val="-2126236328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4529,21 +4541,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2078408040"/>
+        <c:crossAx val="-2129657800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4834,11 +4844,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2095269464"/>
-        <c:axId val="2096070808"/>
+        <c:axId val="-2126203656"/>
+        <c:axId val="-2126197512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095269464"/>
+        <c:axId val="-2126203656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4889,13 +4899,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2096070808"/>
+        <c:crossAx val="-2126197512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4903,7 +4912,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2096070808"/>
+        <c:axId val="-2126197512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4926,21 +4935,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095269464"/>
+        <c:crossAx val="-2126203656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -50961,10 +50968,10 @@
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C23" s="5"/>
+      <c r="C23" s="6"/>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
@@ -51143,10 +51150,10 @@
       </c>
     </row>
     <row r="44" spans="1:14">
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="C44" s="5"/>
+      <c r="C44" s="6"/>
       <c r="N44" t="s">
         <v>367</v>
       </c>
@@ -51436,7 +51443,7 @@
       <c r="A9" t="s">
         <v>382</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>35964948917</v>
       </c>
     </row>
@@ -51476,7 +51483,7 @@
       <c r="A14" t="s">
         <v>387</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>429796769</v>
       </c>
     </row>
@@ -51537,7 +51544,7 @@
       <c r="A19" t="s">
         <v>382</v>
       </c>
-      <c r="B19" s="6">
+      <c r="B19" s="5">
         <v>838087280</v>
       </c>
       <c r="D19">
@@ -51612,7 +51619,7 @@
       <c r="A24" t="s">
         <v>387</v>
       </c>
-      <c r="B24" s="6">
+      <c r="B24" s="5">
         <v>171515084</v>
       </c>
       <c r="D24">
@@ -51659,7 +51666,7 @@
       <c r="A29" t="s">
         <v>382</v>
       </c>
-      <c r="B29" s="6">
+      <c r="B29" s="5">
         <v>43688498181</v>
       </c>
     </row>
@@ -51699,7 +51706,7 @@
       <c r="A34" t="s">
         <v>387</v>
       </c>
-      <c r="B34" s="6">
+      <c r="B34" s="5">
         <v>644595953</v>
       </c>
     </row>
@@ -51763,7 +51770,7 @@
       <c r="A39" t="s">
         <v>382</v>
       </c>
-      <c r="B39" s="6">
+      <c r="B39" s="5">
         <v>95595622</v>
       </c>
       <c r="D39">
@@ -51897,7 +51904,7 @@
       <c r="A52" t="s">
         <v>382</v>
       </c>
-      <c r="B52" s="6">
+      <c r="B52" s="5">
         <v>11486319646</v>
       </c>
     </row>
@@ -51937,7 +51944,7 @@
       <c r="A57" t="s">
         <v>387</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="5">
         <v>1618427411</v>
       </c>
     </row>
@@ -51998,7 +52005,7 @@
       <c r="A62" t="s">
         <v>382</v>
       </c>
-      <c r="B62" s="6">
+      <c r="B62" s="5">
         <v>615476607</v>
       </c>
       <c r="D62">
@@ -52073,7 +52080,7 @@
       <c r="A67" t="s">
         <v>387</v>
       </c>
-      <c r="B67" s="6">
+      <c r="B67" s="5">
         <v>164408118</v>
       </c>
       <c r="D67">
@@ -52120,7 +52127,7 @@
       <c r="A72" t="s">
         <v>382</v>
       </c>
-      <c r="B72" s="6">
+      <c r="B72" s="5">
         <v>10857012358</v>
       </c>
     </row>
@@ -52160,7 +52167,7 @@
       <c r="A77" t="s">
         <v>387</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B77" s="5">
         <v>1282958445</v>
       </c>
     </row>
@@ -52224,7 +52231,7 @@
       <c r="A82" t="s">
         <v>382</v>
       </c>
-      <c r="B82" s="6">
+      <c r="B82" s="5">
         <v>96466402</v>
       </c>
       <c r="D82">
@@ -52299,7 +52306,7 @@
       <c r="A87" t="s">
         <v>387</v>
       </c>
-      <c r="B87" s="6">
+      <c r="B87" s="5">
         <v>21768360</v>
       </c>
       <c r="D87">
@@ -52358,7 +52365,7 @@
       <c r="A95" t="s">
         <v>382</v>
       </c>
-      <c r="B95" s="6">
+      <c r="B95" s="5">
         <v>11615745985</v>
       </c>
     </row>
@@ -52398,7 +52405,7 @@
       <c r="A100" t="s">
         <v>387</v>
       </c>
-      <c r="B100" s="6">
+      <c r="B100" s="5">
         <v>1535863846</v>
       </c>
     </row>
@@ -52459,7 +52466,7 @@
       <c r="A105" t="s">
         <v>382</v>
       </c>
-      <c r="B105" s="6">
+      <c r="B105" s="5">
         <v>611764632</v>
       </c>
       <c r="D105">
@@ -52534,7 +52541,7 @@
       <c r="A110" t="s">
         <v>387</v>
       </c>
-      <c r="B110" s="6">
+      <c r="B110" s="5">
         <v>136722727</v>
       </c>
       <c r="D110">
@@ -52581,7 +52588,7 @@
       <c r="A115" t="s">
         <v>382</v>
       </c>
-      <c r="B115" s="6">
+      <c r="B115" s="5">
         <v>11035198199</v>
       </c>
     </row>
@@ -52621,7 +52628,7 @@
       <c r="A120" t="s">
         <v>387</v>
       </c>
-      <c r="B120" s="6">
+      <c r="B120" s="5">
         <v>1221547545</v>
       </c>
     </row>
@@ -52685,7 +52692,7 @@
       <c r="A125" t="s">
         <v>382</v>
       </c>
-      <c r="B125" s="6">
+      <c r="B125" s="5">
         <v>92619046</v>
       </c>
       <c r="D125">
@@ -52760,7 +52767,7 @@
       <c r="A130" t="s">
         <v>387</v>
       </c>
-      <c r="B130" s="6">
+      <c r="B130" s="5">
         <v>20163082</v>
       </c>
       <c r="D130">
@@ -52819,7 +52826,7 @@
       <c r="A138" t="s">
         <v>382</v>
       </c>
-      <c r="B138" s="6">
+      <c r="B138" s="5">
         <v>24312014337</v>
       </c>
     </row>
@@ -52859,7 +52866,7 @@
       <c r="A143" t="s">
         <v>387</v>
       </c>
-      <c r="B143" s="6">
+      <c r="B143" s="5">
         <v>482530657</v>
       </c>
     </row>
@@ -52920,7 +52927,7 @@
       <c r="A148" t="s">
         <v>382</v>
       </c>
-      <c r="B148" s="6">
+      <c r="B148" s="5">
         <v>346924135</v>
       </c>
       <c r="D148">
@@ -52995,7 +53002,7 @@
       <c r="A153" t="s">
         <v>387</v>
       </c>
-      <c r="B153" s="6">
+      <c r="B153" s="5">
         <v>224590841</v>
       </c>
       <c r="D153">
@@ -53042,7 +53049,7 @@
       <c r="A158" t="s">
         <v>382</v>
       </c>
-      <c r="B158" s="6">
+      <c r="B158" s="5">
         <v>26290370320</v>
       </c>
     </row>
@@ -53082,7 +53089,7 @@
       <c r="A163" t="s">
         <v>387</v>
       </c>
-      <c r="B163" s="6">
+      <c r="B163" s="5">
         <v>737044655</v>
       </c>
     </row>
@@ -53146,7 +53153,7 @@
       <c r="A168" t="s">
         <v>382</v>
       </c>
-      <c r="B168" s="6">
+      <c r="B168" s="5">
         <v>72163711</v>
       </c>
       <c r="D168">
@@ -53221,7 +53228,7 @@
       <c r="A173" t="s">
         <v>387</v>
       </c>
-      <c r="B173" s="6">
+      <c r="B173" s="5">
         <v>15005031</v>
       </c>
       <c r="D173">
@@ -53280,7 +53287,7 @@
       <c r="A181" t="s">
         <v>382</v>
       </c>
-      <c r="B181" s="6">
+      <c r="B181" s="5">
         <v>8901073748</v>
       </c>
     </row>
@@ -53320,7 +53327,7 @@
       <c r="A186" t="s">
         <v>387</v>
       </c>
-      <c r="B186" s="6">
+      <c r="B186" s="5">
         <v>94440678</v>
       </c>
     </row>
@@ -53381,7 +53388,7 @@
       <c r="A191" t="s">
         <v>382</v>
       </c>
-      <c r="B191" s="6">
+      <c r="B191" s="5">
         <v>97866482</v>
       </c>
       <c r="D191">
@@ -53456,7 +53463,7 @@
       <c r="A196" t="s">
         <v>387</v>
       </c>
-      <c r="B196" s="6">
+      <c r="B196" s="5">
         <v>23155604</v>
       </c>
       <c r="D196">
@@ -53503,7 +53510,7 @@
       <c r="A201" t="s">
         <v>382</v>
       </c>
-      <c r="B201" s="6">
+      <c r="B201" s="5">
         <v>8878013174</v>
       </c>
     </row>
@@ -53543,7 +53550,7 @@
       <c r="A206" t="s">
         <v>387</v>
       </c>
-      <c r="B206" s="6">
+      <c r="B206" s="5">
         <v>88717726</v>
       </c>
     </row>
@@ -53607,7 +53614,7 @@
       <c r="A211" t="s">
         <v>382</v>
       </c>
-      <c r="B211" s="6">
+      <c r="B211" s="5">
         <v>86966014</v>
       </c>
       <c r="D211">
@@ -53682,7 +53689,7 @@
       <c r="A216" t="s">
         <v>387</v>
       </c>
-      <c r="B216" s="6">
+      <c r="B216" s="5">
         <v>14022799</v>
       </c>
       <c r="D216">
@@ -53741,7 +53748,7 @@
       <c r="A224" t="s">
         <v>382</v>
       </c>
-      <c r="B224" s="6">
+      <c r="B224" s="5">
         <v>41567957980</v>
       </c>
     </row>
@@ -53781,7 +53788,7 @@
       <c r="A229" t="s">
         <v>387</v>
       </c>
-      <c r="B229" s="6">
+      <c r="B229" s="5">
         <v>193476280</v>
       </c>
     </row>
@@ -53842,7 +53849,7 @@
       <c r="A234" t="s">
         <v>382</v>
       </c>
-      <c r="B234" s="6">
+      <c r="B234" s="5">
         <v>966633346</v>
       </c>
       <c r="D234">
@@ -53917,7 +53924,7 @@
       <c r="A239" t="s">
         <v>387</v>
       </c>
-      <c r="B239" s="6">
+      <c r="B239" s="5">
         <v>98125672</v>
       </c>
       <c r="D239">
@@ -53964,7 +53971,7 @@
       <c r="A244" t="s">
         <v>382</v>
       </c>
-      <c r="B244" s="6">
+      <c r="B244" s="5">
         <v>62819280237</v>
       </c>
     </row>
@@ -54004,7 +54011,7 @@
       <c r="A249" t="s">
         <v>387</v>
       </c>
-      <c r="B249" s="6">
+      <c r="B249" s="5">
         <v>759390978</v>
       </c>
     </row>
@@ -54068,7 +54075,7 @@
       <c r="A254" t="s">
         <v>382</v>
       </c>
-      <c r="B254" s="6">
+      <c r="B254" s="5">
         <v>98093236</v>
       </c>
       <c r="D254">
@@ -54143,7 +54150,7 @@
       <c r="A259" t="s">
         <v>387</v>
       </c>
-      <c r="B259" s="6">
+      <c r="B259" s="5">
         <v>47889800</v>
       </c>
       <c r="D259">
@@ -54202,7 +54209,7 @@
       <c r="A267" t="s">
         <v>382</v>
       </c>
-      <c r="B267" s="6">
+      <c r="B267" s="5">
         <v>24021219601</v>
       </c>
     </row>
@@ -54242,7 +54249,7 @@
       <c r="A272" t="s">
         <v>387</v>
       </c>
-      <c r="B272" s="6">
+      <c r="B272" s="5">
         <v>451906166</v>
       </c>
     </row>
@@ -54303,7 +54310,7 @@
       <c r="A277" t="s">
         <v>382</v>
       </c>
-      <c r="B277" s="6">
+      <c r="B277" s="5">
         <v>345070549</v>
       </c>
       <c r="D277">
@@ -54378,7 +54385,7 @@
       <c r="A282" t="s">
         <v>387</v>
       </c>
-      <c r="B282" s="6">
+      <c r="B282" s="5">
         <v>203807045</v>
       </c>
       <c r="D282">
@@ -54425,7 +54432,7 @@
       <c r="A287" t="s">
         <v>382</v>
       </c>
-      <c r="B287" s="6">
+      <c r="B287" s="5">
         <v>24827276138</v>
       </c>
     </row>
@@ -54465,7 +54472,7 @@
       <c r="A292" t="s">
         <v>387</v>
       </c>
-      <c r="B292" s="6">
+      <c r="B292" s="5">
         <v>610936613</v>
       </c>
     </row>
@@ -54529,7 +54536,7 @@
       <c r="A297" t="s">
         <v>382</v>
       </c>
-      <c r="B297" s="6">
+      <c r="B297" s="5">
         <v>92413777</v>
       </c>
       <c r="D297">
@@ -54604,7 +54611,7 @@
       <c r="A302" t="s">
         <v>387</v>
       </c>
-      <c r="B302" s="6">
+      <c r="B302" s="5">
         <v>64821850</v>
       </c>
       <c r="D302">
@@ -54663,7 +54670,7 @@
       <c r="A310" t="s">
         <v>382</v>
       </c>
-      <c r="B310" s="6">
+      <c r="B310" s="5">
         <v>24912704886</v>
       </c>
     </row>
@@ -54703,7 +54710,7 @@
       <c r="A315" t="s">
         <v>387</v>
       </c>
-      <c r="B315" s="6">
+      <c r="B315" s="5">
         <v>478187115</v>
       </c>
     </row>
@@ -54764,7 +54771,7 @@
       <c r="A320" t="s">
         <v>382</v>
       </c>
-      <c r="B320" s="6">
+      <c r="B320" s="5">
         <v>337725586</v>
       </c>
       <c r="D320">
@@ -54839,7 +54846,7 @@
       <c r="A325" t="s">
         <v>387</v>
       </c>
-      <c r="B325" s="6">
+      <c r="B325" s="5">
         <v>207848124</v>
       </c>
       <c r="D325">
@@ -54886,7 +54893,7 @@
       <c r="A330" t="s">
         <v>382</v>
       </c>
-      <c r="B330" s="6">
+      <c r="B330" s="5">
         <v>29360676887</v>
       </c>
     </row>
@@ -54926,7 +54933,7 @@
       <c r="A335" t="s">
         <v>387</v>
       </c>
-      <c r="B335" s="6">
+      <c r="B335" s="5">
         <v>690340737</v>
       </c>
     </row>
@@ -54990,7 +54997,7 @@
       <c r="A340" t="s">
         <v>382</v>
       </c>
-      <c r="B340" s="6">
+      <c r="B340" s="5">
         <v>93580797</v>
       </c>
       <c r="D340">
@@ -55065,7 +55072,7 @@
       <c r="A345" t="s">
         <v>387</v>
       </c>
-      <c r="B345" s="6">
+      <c r="B345" s="5">
         <v>28588680</v>
       </c>
       <c r="D345">
@@ -55124,7 +55131,7 @@
       <c r="A353" t="s">
         <v>382</v>
       </c>
-      <c r="B353" s="6">
+      <c r="B353" s="5">
         <v>23524849879</v>
       </c>
     </row>
@@ -55164,7 +55171,7 @@
       <c r="A358" t="s">
         <v>387</v>
       </c>
-      <c r="B358" s="6">
+      <c r="B358" s="5">
         <v>464137617</v>
       </c>
     </row>
@@ -55225,7 +55232,7 @@
       <c r="A363" t="s">
         <v>382</v>
       </c>
-      <c r="B363" s="6">
+      <c r="B363" s="5">
         <v>347411697</v>
       </c>
       <c r="D363">
@@ -55300,7 +55307,7 @@
       <c r="A368" t="s">
         <v>387</v>
       </c>
-      <c r="B368" s="6">
+      <c r="B368" s="5">
         <v>207150505</v>
       </c>
       <c r="D368">
@@ -55347,7 +55354,7 @@
       <c r="A373" t="s">
         <v>382</v>
       </c>
-      <c r="B373" s="6">
+      <c r="B373" s="5">
         <v>28624256011</v>
       </c>
     </row>
@@ -55387,7 +55394,7 @@
       <c r="A378" t="s">
         <v>387</v>
       </c>
-      <c r="B378" s="6">
+      <c r="B378" s="5">
         <v>717377380</v>
       </c>
     </row>
@@ -55451,7 +55458,7 @@
       <c r="A383" t="s">
         <v>382</v>
       </c>
-      <c r="B383" s="6">
+      <c r="B383" s="5">
         <v>88203377</v>
       </c>
       <c r="D383">
@@ -55526,7 +55533,7 @@
       <c r="A388" t="s">
         <v>387</v>
       </c>
-      <c r="B388" s="6">
+      <c r="B388" s="5">
         <v>17107313</v>
       </c>
       <c r="D388">
@@ -55585,7 +55592,7 @@
       <c r="A396" t="s">
         <v>382</v>
       </c>
-      <c r="B396" s="6">
+      <c r="B396" s="5">
         <v>8656138117</v>
       </c>
     </row>
@@ -55625,7 +55632,7 @@
       <c r="A401" t="s">
         <v>387</v>
       </c>
-      <c r="B401" s="6">
+      <c r="B401" s="5">
         <v>1072073612</v>
       </c>
     </row>
@@ -55686,7 +55693,7 @@
       <c r="A406" t="s">
         <v>382</v>
       </c>
-      <c r="B406" s="6">
+      <c r="B406" s="5">
         <v>355478944</v>
       </c>
       <c r="D406">
@@ -55761,7 +55768,7 @@
       <c r="A411" t="s">
         <v>387</v>
       </c>
-      <c r="B411" s="6">
+      <c r="B411" s="5">
         <v>38380840</v>
       </c>
       <c r="D411">
@@ -55808,7 +55815,7 @@
       <c r="A416" t="s">
         <v>382</v>
       </c>
-      <c r="B416" s="6">
+      <c r="B416" s="5">
         <v>8447092404</v>
       </c>
     </row>
@@ -55848,7 +55855,7 @@
       <c r="A421" t="s">
         <v>387</v>
       </c>
-      <c r="B421" s="6">
+      <c r="B421" s="5">
         <v>1136961729</v>
       </c>
     </row>
@@ -55912,7 +55919,7 @@
       <c r="A426" t="s">
         <v>382</v>
       </c>
-      <c r="B426" s="6">
+      <c r="B426" s="5">
         <v>90940563</v>
       </c>
       <c r="D426">
@@ -55987,7 +55994,7 @@
       <c r="A431" t="s">
         <v>387</v>
       </c>
-      <c r="B431" s="6">
+      <c r="B431" s="5">
         <v>10507197</v>
       </c>
       <c r="D431">
@@ -56046,7 +56053,7 @@
       <c r="A439" t="s">
         <v>382</v>
       </c>
-      <c r="B439" s="6">
+      <c r="B439" s="5">
         <v>46538713157</v>
       </c>
     </row>
@@ -56086,7 +56093,7 @@
       <c r="A444" t="s">
         <v>387</v>
       </c>
-      <c r="B444" s="6">
+      <c r="B444" s="5">
         <v>407875956</v>
       </c>
     </row>
@@ -56147,7 +56154,7 @@
       <c r="A449" t="s">
         <v>382</v>
       </c>
-      <c r="B449" s="6">
+      <c r="B449" s="5">
         <v>672977880</v>
       </c>
       <c r="D449">
@@ -56222,7 +56229,7 @@
       <c r="A454" t="s">
         <v>387</v>
       </c>
-      <c r="B454" s="6">
+      <c r="B454" s="5">
         <v>128935809</v>
       </c>
       <c r="D454">
@@ -56269,7 +56276,7 @@
       <c r="A459" t="s">
         <v>382</v>
       </c>
-      <c r="B459" s="6">
+      <c r="B459" s="5">
         <v>10921513482</v>
       </c>
     </row>
@@ -56309,7 +56316,7 @@
       <c r="A464" t="s">
         <v>387</v>
       </c>
-      <c r="B464" s="6">
+      <c r="B464" s="5">
         <v>553131292</v>
       </c>
     </row>
@@ -56373,7 +56380,7 @@
       <c r="A469" t="s">
         <v>382</v>
       </c>
-      <c r="B469" s="6">
+      <c r="B469" s="5">
         <v>92463326</v>
       </c>
       <c r="D469">
@@ -56448,7 +56455,7 @@
       <c r="A474" t="s">
         <v>387</v>
       </c>
-      <c r="B474" s="6">
+      <c r="B474" s="5">
         <v>23036661</v>
       </c>
       <c r="D474">
@@ -56507,7 +56514,7 @@
       <c r="A482" t="s">
         <v>382</v>
       </c>
-      <c r="B482" s="6">
+      <c r="B482" s="5">
         <v>24971846029</v>
       </c>
     </row>
@@ -56547,7 +56554,7 @@
       <c r="A487" t="s">
         <v>387</v>
       </c>
-      <c r="B487" s="6">
+      <c r="B487" s="5">
         <v>455540029</v>
       </c>
     </row>
@@ -56608,7 +56615,7 @@
       <c r="A492" t="s">
         <v>382</v>
       </c>
-      <c r="B492" s="6">
+      <c r="B492" s="5">
         <v>332544400</v>
       </c>
       <c r="D492">
@@ -56683,7 +56690,7 @@
       <c r="A497" t="s">
         <v>387</v>
       </c>
-      <c r="B497" s="6">
+      <c r="B497" s="5">
         <v>202807086</v>
       </c>
       <c r="D497">
@@ -56730,7 +56737,7 @@
       <c r="A502" t="s">
         <v>382</v>
       </c>
-      <c r="B502" s="6">
+      <c r="B502" s="5">
         <v>27866840459</v>
       </c>
     </row>
@@ -56770,7 +56777,7 @@
       <c r="A507" t="s">
         <v>387</v>
       </c>
-      <c r="B507" s="6">
+      <c r="B507" s="5">
         <v>655834579</v>
       </c>
     </row>
@@ -56834,7 +56841,7 @@
       <c r="A512" t="s">
         <v>382</v>
       </c>
-      <c r="B512" s="6">
+      <c r="B512" s="5">
         <v>91274910</v>
       </c>
       <c r="D512">
@@ -56909,7 +56916,7 @@
       <c r="A517" t="s">
         <v>387</v>
       </c>
-      <c r="B517" s="6">
+      <c r="B517" s="5">
         <v>23114956</v>
       </c>
       <c r="D517">
@@ -56968,7 +56975,7 @@
       <c r="A525" t="s">
         <v>382</v>
       </c>
-      <c r="B525" s="6">
+      <c r="B525" s="5">
         <v>24941823014</v>
       </c>
     </row>
@@ -57008,7 +57015,7 @@
       <c r="A530" t="s">
         <v>387</v>
       </c>
-      <c r="B530" s="6">
+      <c r="B530" s="5">
         <v>427387594</v>
       </c>
     </row>
@@ -57069,7 +57076,7 @@
       <c r="A535" t="s">
         <v>382</v>
       </c>
-      <c r="B535" s="6">
+      <c r="B535" s="5">
         <v>348692521</v>
       </c>
       <c r="D535">
@@ -57144,7 +57151,7 @@
       <c r="A540" t="s">
         <v>387</v>
       </c>
-      <c r="B540" s="6">
+      <c r="B540" s="5">
         <v>201201085</v>
       </c>
       <c r="D540">
@@ -57191,7 +57198,7 @@
       <c r="A545" t="s">
         <v>382</v>
       </c>
-      <c r="B545" s="6">
+      <c r="B545" s="5">
         <v>26058038910</v>
       </c>
     </row>
@@ -57231,7 +57238,7 @@
       <c r="A550" t="s">
         <v>387</v>
       </c>
-      <c r="B550" s="6">
+      <c r="B550" s="5">
         <v>720794254</v>
       </c>
     </row>
@@ -57295,7 +57302,7 @@
       <c r="A555" t="s">
         <v>382</v>
       </c>
-      <c r="B555" s="6">
+      <c r="B555" s="5">
         <v>95056287</v>
       </c>
       <c r="D555">
@@ -57370,7 +57377,7 @@
       <c r="A560" t="s">
         <v>387</v>
       </c>
-      <c r="B560" s="6">
+      <c r="B560" s="5">
         <v>32417970</v>
       </c>
       <c r="D560">
@@ -57429,7 +57436,7 @@
       <c r="A568" t="s">
         <v>382</v>
       </c>
-      <c r="B568" s="6">
+      <c r="B568" s="5">
         <v>22004097169</v>
       </c>
     </row>
@@ -57469,7 +57476,7 @@
       <c r="A573" t="s">
         <v>387</v>
       </c>
-      <c r="B573" s="6">
+      <c r="B573" s="5">
         <v>436706330</v>
       </c>
     </row>
@@ -57530,7 +57537,7 @@
       <c r="A578" t="s">
         <v>382</v>
       </c>
-      <c r="B578" s="6">
+      <c r="B578" s="5">
         <v>333795432</v>
       </c>
       <c r="D578">
@@ -57605,7 +57612,7 @@
       <c r="A583" t="s">
         <v>387</v>
       </c>
-      <c r="B583" s="6">
+      <c r="B583" s="5">
         <v>206471634</v>
       </c>
       <c r="D583">
@@ -57652,7 +57659,7 @@
       <c r="A588" t="s">
         <v>382</v>
       </c>
-      <c r="B588" s="6">
+      <c r="B588" s="5">
         <v>27784248353</v>
       </c>
     </row>
@@ -57692,7 +57699,7 @@
       <c r="A593" t="s">
         <v>387</v>
       </c>
-      <c r="B593" s="6">
+      <c r="B593" s="5">
         <v>709776415</v>
       </c>
     </row>
@@ -57756,7 +57763,7 @@
       <c r="A598" t="s">
         <v>382</v>
       </c>
-      <c r="B598" s="6">
+      <c r="B598" s="5">
         <v>91271352</v>
       </c>
       <c r="D598">
@@ -57831,7 +57838,7 @@
       <c r="A603" t="s">
         <v>387</v>
       </c>
-      <c r="B603" s="6">
+      <c r="B603" s="5">
         <v>15027046</v>
       </c>
       <c r="D603">
@@ -57890,7 +57897,7 @@
       <c r="A611" t="s">
         <v>382</v>
       </c>
-      <c r="B611" s="6">
+      <c r="B611" s="5">
         <v>49291675936</v>
       </c>
     </row>
@@ -57930,7 +57937,7 @@
       <c r="A616" t="s">
         <v>387</v>
       </c>
-      <c r="B616" s="6">
+      <c r="B616" s="5">
         <v>930921487</v>
       </c>
     </row>
@@ -57991,7 +57998,7 @@
       <c r="A621" t="s">
         <v>382</v>
       </c>
-      <c r="B621" s="6">
+      <c r="B621" s="5">
         <v>871181822</v>
       </c>
       <c r="D621">
@@ -58066,7 +58073,7 @@
       <c r="A626" t="s">
         <v>387</v>
       </c>
-      <c r="B626" s="6">
+      <c r="B626" s="5">
         <v>47801807</v>
       </c>
       <c r="D626">
@@ -58113,7 +58120,7 @@
       <c r="A631" t="s">
         <v>382</v>
       </c>
-      <c r="B631" s="6">
+      <c r="B631" s="5">
         <v>42302503453</v>
       </c>
     </row>
@@ -58153,7 +58160,7 @@
       <c r="A636" t="s">
         <v>387</v>
       </c>
-      <c r="B636" s="6">
+      <c r="B636" s="5">
         <v>181580965</v>
       </c>
     </row>
@@ -58217,7 +58224,7 @@
       <c r="A641" t="s">
         <v>382</v>
       </c>
-      <c r="B641" s="6">
+      <c r="B641" s="5">
         <v>88927097</v>
       </c>
       <c r="D641">
@@ -58292,7 +58299,7 @@
       <c r="A646" t="s">
         <v>387</v>
       </c>
-      <c r="B646" s="6">
+      <c r="B646" s="5">
         <v>34889217</v>
       </c>
       <c r="D646">
@@ -58318,7 +58325,7 @@
   <dimension ref="A1:H200"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1048576"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58330,7 +58337,7 @@
     <col min="5" max="5" width="25.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>370</v>
       </c>
@@ -58343,8 +58350,11 @@
       <c r="D1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>393</v>
       </c>
@@ -58357,8 +58367,12 @@
       <c r="D2">
         <v>59655557477</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="E2" s="7">
+        <f>+(D2-C2)/C2</f>
+        <v>-0.38387281875812318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="B3" t="s">
         <v>380</v>
       </c>
@@ -58368,8 +58382,12 @@
       <c r="D3">
         <v>65515252443</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E10" si="0">+(D3-C3)/C3</f>
+        <v>-0.17878799405536577</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="B4" t="s">
         <v>381</v>
       </c>
@@ -58379,8 +58397,12 @@
       <c r="D4">
         <v>21922349884</v>
       </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>-0.50903848456421774</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="B5" t="s">
         <v>382</v>
       </c>
@@ -58390,8 +58412,12 @@
       <c r="D5">
         <v>43592902559</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.24101330228381426</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="B6" t="s">
         <v>383</v>
       </c>
@@ -58401,8 +58427,12 @@
       <c r="D6">
         <v>1656647554</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.70871146080135294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="B7" t="s">
         <v>384</v>
       </c>
@@ -58412,8 +58442,12 @@
       <c r="D7">
         <v>240660405</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>0.22217470626403807</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="B8" t="s">
         <v>385</v>
       </c>
@@ -58423,8 +58457,12 @@
       <c r="D8">
         <v>304661604</v>
       </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.10117681553204143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="B9" t="s">
         <v>386</v>
       </c>
@@ -58434,8 +58472,12 @@
       <c r="D9">
         <v>470288218</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E9" s="7">
+        <f t="shared" si="0"/>
+        <v>0.97876205393123816</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="B10" t="s">
         <v>387</v>
       </c>
@@ -58445,8 +58487,12 @@
       <c r="D10">
         <v>641037327</v>
       </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="E10" s="7">
+        <f t="shared" si="0"/>
+        <v>1.4819310242613601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>394</v>
       </c>
@@ -58459,8 +58505,12 @@
       <c r="D12">
         <v>14965064917</v>
       </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="E12" s="7">
+        <f>+(D12-C12)/C12</f>
+        <v>-2.3814206795224522E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="B13" t="s">
         <v>380</v>
       </c>
@@ -58470,8 +58520,12 @@
       <c r="D13">
         <v>11482700125</v>
       </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="E13" s="7">
+        <f t="shared" ref="E13:E20" si="1">+(D13-C13)/C13</f>
+        <v>-2.7417828017801498E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="B14" t="s">
         <v>381</v>
       </c>
@@ -58481,8 +58535,12 @@
       <c r="D14">
         <v>722154169</v>
       </c>
-    </row>
-    <row r="15" spans="1:4">
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.22810746835580353</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="B15" t="s">
         <v>382</v>
       </c>
@@ -58492,8 +58550,12 @@
       <c r="D15">
         <v>10760545956</v>
       </c>
-    </row>
-    <row r="16" spans="1:4">
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
+        <v>-1.0146138860095816E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="B16" t="s">
         <v>383</v>
       </c>
@@ -58502,6 +58564,10 @@
       </c>
       <c r="D16">
         <v>3275414789</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="1"/>
+        <v>-3.0618106425754452E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -58514,6 +58580,10 @@
       <c r="D17">
         <v>1496878521</v>
       </c>
+      <c r="E17" s="7">
+        <f t="shared" si="1"/>
+        <v>-2.5607409281081673E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:8">
       <c r="B18" t="s">
@@ -58525,6 +58595,10 @@
       <c r="D18">
         <v>303577983</v>
       </c>
+      <c r="E18" s="7">
+        <f t="shared" si="1"/>
+        <v>7.9342669760418899E-2</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
       <c r="B19" t="s">
@@ -58536,6 +58610,10 @@
       <c r="D19">
         <v>213768200</v>
       </c>
+      <c r="E19" s="7">
+        <f t="shared" si="1"/>
+        <v>0.9909285464564368</v>
+      </c>
     </row>
     <row r="20" spans="1:8">
       <c r="B20" t="s">
@@ -58547,6 +58625,10 @@
       <c r="D20">
         <v>1261190085</v>
       </c>
+      <c r="E20" s="7">
+        <f t="shared" si="1"/>
+        <v>-0.1326180532323927</v>
+      </c>
     </row>
     <row r="22" spans="1:8">
       <c r="A22" t="s">
@@ -58561,6 +58643,10 @@
       <c r="D22">
         <v>14724989219</v>
       </c>
+      <c r="E22" s="7">
+        <f>+(D22-C22)/C22</f>
+        <v>-1.5480145274010778E-2</v>
+      </c>
     </row>
     <row r="23" spans="1:8">
       <c r="B23" t="s">
@@ -58572,6 +58658,10 @@
       <c r="D23">
         <v>11653254818</v>
       </c>
+      <c r="E23" s="7">
+        <f t="shared" ref="E23:E30" si="2">+(D23-C23)/C23</f>
+        <v>-1.2334921415967771E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:8">
       <c r="B24" t="s">
@@ -58583,6 +58673,10 @@
       <c r="D24">
         <v>710675665</v>
       </c>
+      <c r="E24" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.10585536740872782</v>
+      </c>
     </row>
     <row r="25" spans="1:8">
       <c r="B25" t="s">
@@ -58594,6 +58688,10 @@
       <c r="D25">
         <v>10942579153</v>
       </c>
+      <c r="E25" s="7">
+        <f t="shared" si="2"/>
+        <v>-5.5799985505482529E-3</v>
+      </c>
     </row>
     <row r="26" spans="1:8">
       <c r="B26" t="s">
@@ -58605,6 +58703,10 @@
       <c r="D26">
         <v>3187216172</v>
       </c>
+      <c r="E26" s="7">
+        <f t="shared" si="2"/>
+        <v>-3.9513398307099545E-2</v>
+      </c>
     </row>
     <row r="27" spans="1:8">
       <c r="B27" t="s">
@@ -58616,6 +58718,10 @@
       <c r="D27">
         <v>1563597947</v>
       </c>
+      <c r="E27" s="7">
+        <f t="shared" si="2"/>
+        <v>2.6367251105470398E-2</v>
+      </c>
     </row>
     <row r="28" spans="1:8">
       <c r="B28" t="s">
@@ -58627,6 +58733,10 @@
       <c r="D28">
         <v>297999605</v>
       </c>
+      <c r="E28" s="7">
+        <f t="shared" si="2"/>
+        <v>6.8858452781293183E-2</v>
+      </c>
       <c r="H28" t="s">
         <v>405</v>
       </c>
@@ -58641,6 +58751,10 @@
       <c r="D29">
         <v>124234157</v>
       </c>
+      <c r="E29" s="7">
+        <f t="shared" si="2"/>
+        <v>6.2169133801028925E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:8">
       <c r="B30" t="s">
@@ -58652,6 +58766,10 @@
       <c r="D30">
         <v>1201384463</v>
       </c>
+      <c r="E30" s="7">
+        <f t="shared" si="2"/>
+        <v>-0.14134146535650491</v>
+      </c>
     </row>
     <row r="32" spans="1:8">
       <c r="A32" t="s">
@@ -58666,8 +58784,12 @@
       <c r="D32">
         <v>70982477581</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" s="7">
+        <f>+(D32-C32)/C32</f>
+        <v>0.32816530409532135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="B33" t="s">
         <v>380</v>
       </c>
@@ -58677,8 +58799,12 @@
       <c r="D33">
         <v>69168831575</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" s="7">
+        <f t="shared" ref="E33:E40" si="3">+(D33-C33)/C33</f>
+        <v>0.30964176301586588</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="B34" t="s">
         <v>381</v>
       </c>
@@ -58688,8 +58814,12 @@
       <c r="D34">
         <v>42950624966</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" s="7">
+        <f t="shared" si="3"/>
+        <v>0.48875713907517143</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="B35" t="s">
         <v>382</v>
       </c>
@@ -58699,8 +58829,12 @@
       <c r="D35">
         <v>26218206609</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" s="7">
+        <f t="shared" si="3"/>
+        <v>9.4016604486302613E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="B36" t="s">
         <v>383</v>
       </c>
@@ -58710,8 +58844,12 @@
       <c r="D36">
         <v>1325371393</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" s="7">
+        <f t="shared" si="3"/>
+        <v>0.78561115125110492</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="B37" t="s">
         <v>384</v>
       </c>
@@ -58721,8 +58859,12 @@
       <c r="D37">
         <v>100812372</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" s="7">
+        <f t="shared" si="3"/>
+        <v>-2.762559579920992E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="B38" t="s">
         <v>385</v>
       </c>
@@ -58732,8 +58874,12 @@
       <c r="D38">
         <v>327197827</v>
       </c>
-    </row>
-    <row r="39" spans="1:4">
+      <c r="E38" s="7">
+        <f t="shared" si="3"/>
+        <v>0.32728146971696959</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="B39" t="s">
         <v>386</v>
       </c>
@@ -58743,8 +58889,12 @@
       <c r="D39">
         <v>175321570</v>
       </c>
-    </row>
-    <row r="40" spans="1:4">
+      <c r="E39" s="7">
+        <f t="shared" si="3"/>
+        <v>0.30722611228030783</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="B40" t="s">
         <v>387</v>
       </c>
@@ -58754,8 +58904,12 @@
       <c r="D40">
         <v>722039624</v>
       </c>
-    </row>
-    <row r="42" spans="1:4">
+      <c r="E40" s="7">
+        <f t="shared" si="3"/>
+        <v>1.799256179976495</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>396</v>
       </c>
@@ -58768,8 +58922,12 @@
       <c r="D42">
         <v>11763313646</v>
       </c>
-    </row>
-    <row r="43" spans="1:4">
+      <c r="E42" s="7">
+        <f>+(D42-C42)/C42</f>
+        <v>1.5029508263153236E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="B43" t="s">
         <v>380</v>
       </c>
@@ -58779,8 +58937,12 @@
       <c r="D43">
         <v>11109359710</v>
       </c>
-    </row>
-    <row r="44" spans="1:4">
+      <c r="E43" s="7">
+        <f t="shared" ref="E43:E50" si="4">+(D43-C43)/C43</f>
+        <v>1.2092554005434134E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="B44" t="s">
         <v>381</v>
       </c>
@@ -58790,8 +58952,12 @@
       <c r="D44">
         <v>2318312550</v>
       </c>
-    </row>
-    <row r="45" spans="1:4">
+      <c r="E44" s="7">
+        <f t="shared" si="4"/>
+        <v>6.6667154316600363E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="B45" t="s">
         <v>382</v>
       </c>
@@ -58801,8 +58967,12 @@
       <c r="D45">
         <v>8791047160</v>
       </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="E45" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.3813267860868289E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="B46" t="s">
         <v>383</v>
       </c>
@@ -58812,8 +58982,12 @@
       <c r="D46">
         <v>721744357</v>
       </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="E46" s="7">
+        <f t="shared" si="4"/>
+        <v>0.10206115371794365</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="B47" t="s">
         <v>384</v>
       </c>
@@ -58823,8 +58997,12 @@
       <c r="D47">
         <v>566266312</v>
       </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="E47" s="7">
+        <f t="shared" si="4"/>
+        <v>0.11978403505156668</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="B48" t="s">
         <v>385</v>
       </c>
@@ -58834,8 +59012,12 @@
       <c r="D48">
         <v>19656402</v>
       </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="E48" s="7">
+        <f t="shared" si="4"/>
+        <v>0.22391806790775748</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="B49" t="s">
         <v>386</v>
       </c>
@@ -58845,8 +59027,12 @@
       <c r="D49">
         <v>61126716</v>
       </c>
-    </row>
-    <row r="50" spans="1:4">
+      <c r="E49" s="7">
+        <f t="shared" si="4"/>
+        <v>-1.1955463936562485E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="B50" t="s">
         <v>387</v>
       </c>
@@ -58856,8 +59042,12 @@
       <c r="D50">
         <v>74694927</v>
       </c>
-    </row>
-    <row r="52" spans="1:4">
+      <c r="E50" s="7">
+        <f t="shared" si="4"/>
+        <v>4.7834038862048456E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>397</v>
       </c>
@@ -58870,8 +59060,12 @@
       <c r="D52">
         <v>68296039986</v>
       </c>
-    </row>
-    <row r="53" spans="1:4">
+      <c r="E52" s="7">
+        <f>+(D52-C52)/C52</f>
+        <v>-0.19626435398544659</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="B53" t="s">
         <v>380</v>
       </c>
@@ -58881,8 +59075,12 @@
       <c r="D53">
         <v>84677754491</v>
       </c>
-    </row>
-    <row r="54" spans="1:4">
+      <c r="E53" s="7">
+        <f t="shared" ref="E53:E60" si="5">+(D53-C53)/C53</f>
+        <v>5.3589268758481405E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="B54" t="s">
         <v>381</v>
       </c>
@@ -58892,8 +59090,12 @@
       <c r="D54">
         <v>21956567490</v>
       </c>
-    </row>
-    <row r="55" spans="1:4">
+      <c r="E54" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.4479032566074837</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="B55" t="s">
         <v>382</v>
       </c>
@@ -58903,8 +59105,12 @@
       <c r="D55">
         <v>62721187001</v>
       </c>
-    </row>
-    <row r="56" spans="1:4">
+      <c r="E55" s="7">
+        <f t="shared" si="5"/>
+        <v>0.54480642113032396</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="B56" t="s">
         <v>383</v>
       </c>
@@ -58914,8 +59120,12 @@
       <c r="D56">
         <v>1703931287</v>
       </c>
-    </row>
-    <row r="57" spans="1:4">
+      <c r="E56" s="7">
+        <f t="shared" si="5"/>
+        <v>1.1497923084409802</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="B57" t="s">
         <v>384</v>
       </c>
@@ -58925,8 +59135,12 @@
       <c r="D57">
         <v>105032789</v>
       </c>
-    </row>
-    <row r="58" spans="1:4">
+      <c r="E57" s="7">
+        <f t="shared" si="5"/>
+        <v>-0.42578990552228707</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="B58" t="s">
         <v>385</v>
       </c>
@@ -58936,8 +59150,12 @@
       <c r="D58">
         <v>300189628</v>
       </c>
-    </row>
-    <row r="59" spans="1:4">
+      <c r="E58" s="7">
+        <f t="shared" si="5"/>
+        <v>4.4728193346153772E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="B59" t="s">
         <v>386</v>
       </c>
@@ -58947,8 +59165,12 @@
       <c r="D59">
         <v>587207692</v>
       </c>
-    </row>
-    <row r="60" spans="1:4">
+      <c r="E59" s="7">
+        <f t="shared" si="5"/>
+        <v>1.5868454105265264</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="B60" t="s">
         <v>387</v>
       </c>
@@ -58958,8 +59180,12 @@
       <c r="D60">
         <v>711501178</v>
       </c>
-    </row>
-    <row r="62" spans="1:4">
+      <c r="E60" s="7">
+        <f t="shared" si="5"/>
+        <v>6.4619469442711894</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>398</v>
       </c>
@@ -58972,8 +59198,12 @@
       <c r="D62">
         <v>67754833523</v>
       </c>
-    </row>
-    <row r="63" spans="1:4">
+      <c r="E62" s="7">
+        <f>+(D62-C62)/C62</f>
+        <v>0.30760068893590037</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="B63" t="s">
         <v>380</v>
       </c>
@@ -58983,8 +59213,12 @@
       <c r="D63">
         <v>66115820405</v>
       </c>
-    </row>
-    <row r="64" spans="1:4">
+      <c r="E63" s="7">
+        <f t="shared" ref="E63:E70" si="6">+(D63-C63)/C63</f>
+        <v>0.28451237295199011</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="B64" t="s">
         <v>381</v>
       </c>
@@ -58994,8 +59228,12 @@
       <c r="D64">
         <v>41380958044</v>
       </c>
-    </row>
-    <row r="65" spans="1:4">
+      <c r="E64" s="7">
+        <f t="shared" si="6"/>
+        <v>0.48877089819205799</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="B65" t="s">
         <v>382</v>
       </c>
@@ -59005,8 +59243,12 @@
       <c r="D65">
         <v>24734862361</v>
       </c>
-    </row>
-    <row r="66" spans="1:4">
+      <c r="E65" s="7">
+        <f t="shared" si="6"/>
+        <v>4.4716448890178243E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="B66" t="s">
         <v>383</v>
       </c>
@@ -59016,8 +59258,12 @@
       <c r="D66">
         <v>1139740303</v>
       </c>
-    </row>
-    <row r="67" spans="1:4">
+      <c r="E66" s="7">
+        <f t="shared" si="6"/>
+        <v>0.60831797411290323</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="B67" t="s">
         <v>384</v>
       </c>
@@ -59027,8 +59273,12 @@
       <c r="D67">
         <v>153626898</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
+      <c r="E67" s="7">
+        <f t="shared" si="6"/>
+        <v>0.55686288196734524</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="B68" t="s">
         <v>385</v>
       </c>
@@ -59038,8 +59288,12 @@
       <c r="D68">
         <v>296036920</v>
       </c>
-    </row>
-    <row r="69" spans="1:4">
+      <c r="E68" s="7">
+        <f t="shared" si="6"/>
+        <v>0.23902388428377569</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="B69" t="s">
         <v>386</v>
       </c>
@@ -59049,8 +59303,12 @@
       <c r="D69">
         <v>143961722</v>
       </c>
-    </row>
-    <row r="70" spans="1:4">
+      <c r="E69" s="7">
+        <f t="shared" si="6"/>
+        <v>0.17089918288221179</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="B70" t="s">
         <v>387</v>
       </c>
@@ -59060,8 +59318,12 @@
       <c r="D70">
         <v>546114763</v>
       </c>
-    </row>
-    <row r="72" spans="1:4">
+      <c r="E70" s="7">
+        <f t="shared" si="6"/>
+        <v>1.2011958800934244</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>399</v>
       </c>
@@ -59074,8 +59336,12 @@
       <c r="D72">
         <v>74790930551</v>
       </c>
-    </row>
-    <row r="73" spans="1:4">
+      <c r="E72" s="7">
+        <f>+(D72-C72)/C72</f>
+        <v>0.40035943287798692</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="B73" t="s">
         <v>380</v>
       </c>
@@ -59085,8 +59351,12 @@
       <c r="D73">
         <v>75177236176</v>
       </c>
-    </row>
-    <row r="74" spans="1:4">
+      <c r="E73" s="7">
+        <f t="shared" ref="E73:E80" si="7">+(D73-C73)/C73</f>
+        <v>0.40304221865241024</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="B74" t="s">
         <v>381</v>
       </c>
@@ -59096,8 +59366,12 @@
       <c r="D74">
         <v>45910140086</v>
       </c>
-    </row>
-    <row r="75" spans="1:4">
+      <c r="E74" s="7">
+        <f t="shared" si="7"/>
+        <v>0.58274735643380937</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="B75" t="s">
         <v>382</v>
       </c>
@@ -59107,8 +59381,12 @@
       <c r="D75">
         <v>29267096090</v>
       </c>
-    </row>
-    <row r="76" spans="1:4">
+      <c r="E75" s="7">
+        <f t="shared" si="7"/>
+        <v>0.19093065075338639</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="B76" t="s">
         <v>383</v>
       </c>
@@ -59118,8 +59396,12 @@
       <c r="D76">
         <v>1316875442</v>
       </c>
-    </row>
-    <row r="77" spans="1:4">
+      <c r="E76" s="7">
+        <f t="shared" si="7"/>
+        <v>0.78994459369135839</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="B77" t="s">
         <v>384</v>
       </c>
@@ -59129,8 +59411,12 @@
       <c r="D77">
         <v>128422641</v>
       </c>
-    </row>
-    <row r="78" spans="1:4">
+      <c r="E77" s="7">
+        <f t="shared" si="7"/>
+        <v>0.30784483213736191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="B78" t="s">
         <v>385</v>
       </c>
@@ -59140,8 +59426,12 @@
       <c r="D78">
         <v>328485626</v>
       </c>
-    </row>
-    <row r="79" spans="1:4">
+      <c r="E78" s="7">
+        <f t="shared" si="7"/>
+        <v>0.40750916416400446</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="B79" t="s">
         <v>386</v>
       </c>
@@ -59151,8 +59441,12 @@
       <c r="D79">
         <v>198215118</v>
       </c>
-    </row>
-    <row r="80" spans="1:4">
+      <c r="E79" s="7">
+        <f t="shared" si="7"/>
+        <v>0.48150055620796234</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="B80" t="s">
         <v>387</v>
       </c>
@@ -59162,8 +59456,12 @@
       <c r="D80">
         <v>661752057</v>
       </c>
-    </row>
-    <row r="82" spans="1:4">
+      <c r="E80" s="7">
+        <f t="shared" si="7"/>
+        <v>1.4478602015644868</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>28</v>
       </c>
@@ -59176,8 +59474,12 @@
       <c r="D82">
         <v>78209961199</v>
       </c>
-    </row>
-    <row r="83" spans="1:4">
+      <c r="E82" s="7">
+        <f>+(D82-C82)/C82</f>
+        <v>0.44919484442667712</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="B83" t="s">
         <v>380</v>
       </c>
@@ -59187,8 +59489,12 @@
       <c r="D83">
         <v>75608838999</v>
       </c>
-    </row>
-    <row r="84" spans="1:4">
+      <c r="E83" s="7">
+        <f t="shared" ref="E83:E90" si="8">+(D83-C83)/C83</f>
+        <v>0.44977063674646239</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="B84" t="s">
         <v>381</v>
       </c>
@@ -59198,8 +59504,12 @@
       <c r="D84">
         <v>47072786365</v>
       </c>
-    </row>
-    <row r="85" spans="1:4">
+      <c r="E84" s="7">
+        <f t="shared" si="8"/>
+        <v>0.62460911677382269</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="B85" t="s">
         <v>382</v>
       </c>
@@ -59209,8 +59519,12 @@
       <c r="D85">
         <v>28536052634</v>
       </c>
-    </row>
-    <row r="86" spans="1:4">
+      <c r="E85" s="7">
+        <f t="shared" si="8"/>
+        <v>0.23119960065998979</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="B86" t="s">
         <v>383</v>
       </c>
@@ -59220,8 +59534,12 @@
       <c r="D86">
         <v>1339213903</v>
       </c>
-    </row>
-    <row r="87" spans="1:4">
+      <c r="E86" s="7">
+        <f t="shared" si="8"/>
+        <v>0.85200576053552191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="B87" t="s">
         <v>384</v>
       </c>
@@ -59231,8 +59549,12 @@
       <c r="D87">
         <v>168751108</v>
       </c>
-    </row>
-    <row r="88" spans="1:4">
+      <c r="E87" s="7">
+        <f t="shared" si="8"/>
+        <v>0.69917789027128618</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="B88" t="s">
         <v>385</v>
       </c>
@@ -59242,8 +59564,12 @@
       <c r="D88">
         <v>338217643</v>
       </c>
-    </row>
-    <row r="89" spans="1:4">
+      <c r="E88" s="7">
+        <f t="shared" si="8"/>
+        <v>0.44683704766766247</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="B89" t="s">
         <v>386</v>
       </c>
@@ -59253,8 +59579,12 @@
       <c r="D89">
         <v>131975085</v>
       </c>
-    </row>
-    <row r="90" spans="1:4">
+      <c r="E89" s="7">
+        <f t="shared" si="8"/>
+        <v>-8.0898106135577057E-3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="B90" t="s">
         <v>387</v>
       </c>
@@ -59264,8 +59594,12 @@
       <c r="D90">
         <v>700270067</v>
       </c>
-    </row>
-    <row r="92" spans="1:4">
+      <c r="E90" s="7">
+        <f t="shared" si="8"/>
+        <v>1.7249229019702748</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>400</v>
       </c>
@@ -59278,8 +59612,12 @@
       <c r="D92">
         <v>11676938139</v>
       </c>
-    </row>
-    <row r="93" spans="1:4">
+      <c r="E92" s="7">
+        <f>+(D92-C92)/C92</f>
+        <v>-1.3494306970266781E-2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="B93" t="s">
         <v>380</v>
       </c>
@@ -59289,8 +59627,12 @@
       <c r="D93">
         <v>8632570910</v>
       </c>
-    </row>
-    <row r="94" spans="1:4">
+      <c r="E93" s="7">
+        <f t="shared" ref="E93:E100" si="9">+(D93-C93)/C93</f>
+        <v>5.5916678900905618E-3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="B94" t="s">
         <v>381</v>
       </c>
@@ -59300,8 +59642,12 @@
       <c r="D94">
         <v>276419069</v>
       </c>
-    </row>
-    <row r="95" spans="1:4">
+      <c r="E94" s="7">
+        <f t="shared" si="9"/>
+        <v>-2.6383778201517393E-2</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="B95" t="s">
         <v>382</v>
       </c>
@@ -59311,8 +59657,12 @@
       <c r="D95">
         <v>8356151841</v>
       </c>
-    </row>
-    <row r="96" spans="1:4">
+      <c r="E95" s="7">
+        <f t="shared" si="9"/>
+        <v>6.6853326758077218E-3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="B96" t="s">
         <v>383</v>
       </c>
@@ -59322,8 +59672,12 @@
       <c r="D96">
         <v>3112592305</v>
       </c>
-    </row>
-    <row r="97" spans="1:4">
+      <c r="E96" s="7">
+        <f t="shared" si="9"/>
+        <v>-1.0843869685961134E-2</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="B97" t="s">
         <v>384</v>
       </c>
@@ -59333,8 +59687,12 @@
       <c r="D97">
         <v>1564029501</v>
       </c>
-    </row>
-    <row r="98" spans="1:4">
+      <c r="E97" s="7">
+        <f t="shared" si="9"/>
+        <v>-0.12831518611185364</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="B98" t="s">
         <v>385</v>
       </c>
@@ -59344,8 +59702,12 @@
       <c r="D98">
         <v>167029967</v>
       </c>
-    </row>
-    <row r="99" spans="1:4">
+      <c r="E98" s="7">
+        <f t="shared" si="9"/>
+        <v>0.45669402097235146</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="B99" t="s">
         <v>386</v>
       </c>
@@ -59355,8 +59717,12 @@
       <c r="D99">
         <v>255078305</v>
       </c>
-    </row>
-    <row r="100" spans="1:4">
+      <c r="E99" s="7">
+        <f t="shared" si="9"/>
+        <v>0.24978334552085976</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="B100" t="s">
         <v>387</v>
       </c>
@@ -59366,8 +59732,12 @@
       <c r="D100">
         <v>1126454532</v>
       </c>
-    </row>
-    <row r="102" spans="1:4">
+      <c r="E100" s="7">
+        <f t="shared" si="9"/>
+        <v>8.9738230267900135E-2</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="2" t="s">
         <v>401</v>
       </c>
@@ -59380,8 +59750,12 @@
       <c r="D102">
         <v>68200644646</v>
       </c>
-    </row>
-    <row r="103" spans="1:4">
+      <c r="E102" s="7">
+        <f>+(D102-C102)/C102</f>
+        <v>-0.15062381620305787</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
       <c r="A103" s="2"/>
       <c r="B103" t="s">
         <v>380</v>
@@ -59392,8 +59766,12 @@
       <c r="D103">
         <v>43434705715</v>
       </c>
-    </row>
-    <row r="104" spans="1:4">
+      <c r="E103" s="7">
+        <f t="shared" ref="E103:E110" si="10">+(D103-C103)/C103</f>
+        <v>-0.48658127523743228</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5">
       <c r="A104" s="2"/>
       <c r="B104" t="s">
         <v>381</v>
@@ -59404,8 +59782,12 @@
       <c r="D104">
         <v>32605655559</v>
       </c>
-    </row>
-    <row r="105" spans="1:4">
+      <c r="E104" s="7">
+        <f t="shared" si="10"/>
+        <v>-0.15819996172998632</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5">
       <c r="A105" s="2"/>
       <c r="B105" t="s">
         <v>382</v>
@@ -59416,8 +59798,12 @@
       <c r="D105">
         <v>10829050156</v>
       </c>
-    </row>
-    <row r="106" spans="1:4">
+      <c r="E105" s="7">
+        <f t="shared" si="10"/>
+        <v>-0.7638967283398076</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5">
       <c r="A106" s="2"/>
       <c r="B106" t="s">
         <v>383</v>
@@ -59428,8 +59814,12 @@
       <c r="D106">
         <v>1385685293</v>
       </c>
-    </row>
-    <row r="107" spans="1:4">
+      <c r="E106" s="7">
+        <f t="shared" si="10"/>
+        <v>0.44196796152733286</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5">
       <c r="A107" s="2"/>
       <c r="B107" t="s">
         <v>384</v>
@@ -59440,8 +59830,12 @@
       <c r="D107">
         <v>227379057</v>
       </c>
-    </row>
-    <row r="108" spans="1:4">
+      <c r="E107" s="7">
+        <f t="shared" si="10"/>
+        <v>0.37471421871519445</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
       <c r="A108" s="2"/>
       <c r="B108" t="s">
         <v>385</v>
@@ -59452,8 +59846,12 @@
       <c r="D108">
         <v>318768647</v>
       </c>
-    </row>
-    <row r="109" spans="1:4">
+      <c r="E108" s="7">
+        <f t="shared" si="10"/>
+        <v>0.15206705657949041</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
       <c r="A109" s="2"/>
       <c r="B109" t="s">
         <v>386</v>
@@ -59464,8 +59862,12 @@
       <c r="D109">
         <v>309442958</v>
       </c>
-    </row>
-    <row r="110" spans="1:4">
+      <c r="E109" s="7">
+        <f t="shared" si="10"/>
+        <v>0.28969894986566652</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5">
       <c r="A110" s="2"/>
       <c r="B110" t="s">
         <v>387</v>
@@ -59476,11 +59878,15 @@
       <c r="D110">
         <v>530094631</v>
       </c>
-    </row>
-    <row r="111" spans="1:4">
+      <c r="E110" s="7">
+        <f t="shared" si="10"/>
+        <v>0.90038844067863777</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:4">
+    <row r="112" spans="1:5">
       <c r="A112" s="2" t="s">
         <v>402</v>
       </c>
@@ -59493,8 +59899,12 @@
       <c r="D112">
         <v>69366081699</v>
       </c>
-    </row>
-    <row r="113" spans="1:4">
+      <c r="E112" s="7">
+        <f>+(D112-C112)/C112</f>
+        <v>0.29816313412242007</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5">
       <c r="A113" s="2"/>
       <c r="B113" t="s">
         <v>380</v>
@@ -59505,8 +59915,12 @@
       <c r="D113">
         <v>68985363063</v>
       </c>
-    </row>
-    <row r="114" spans="1:4">
+      <c r="E113" s="7">
+        <f t="shared" ref="E113:E120" si="11">+(D113-C113)/C113</f>
+        <v>0.2977890724158147</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5">
       <c r="A114" s="2"/>
       <c r="B114" t="s">
         <v>381</v>
@@ -59517,8 +59931,12 @@
       <c r="D114">
         <v>41209797514</v>
       </c>
-    </row>
-    <row r="115" spans="1:4">
+      <c r="E114" s="7">
+        <f t="shared" si="11"/>
+        <v>0.44510770348197937</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5">
       <c r="A115" s="2"/>
       <c r="B115" t="s">
         <v>382</v>
@@ -59529,8 +59947,12 @@
       <c r="D115">
         <v>27775565549</v>
       </c>
-    </row>
-    <row r="116" spans="1:4">
+      <c r="E115" s="7">
+        <f t="shared" si="11"/>
+        <v>0.127287046005747</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5">
       <c r="A116" s="2"/>
       <c r="B116" t="s">
         <v>383</v>
@@ -59541,8 +59963,12 @@
       <c r="D116">
         <v>1277191784</v>
       </c>
-    </row>
-    <row r="117" spans="1:4">
+      <c r="E116" s="7">
+        <f t="shared" si="11"/>
+        <v>0.80647749685558168</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
       <c r="A117" s="2"/>
       <c r="B117" t="s">
         <v>384</v>
@@ -59553,8 +59979,12 @@
       <c r="D117">
         <v>144920588</v>
       </c>
-    </row>
-    <row r="118" spans="1:4">
+      <c r="E117" s="7">
+        <f t="shared" si="11"/>
+        <v>0.57423581274612678</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5">
       <c r="A118" s="2"/>
       <c r="B118" t="s">
         <v>385</v>
@@ -59565,8 +59995,12 @@
       <c r="D118">
         <v>321355951</v>
       </c>
-    </row>
-    <row r="119" spans="1:4">
+      <c r="E118" s="7">
+        <f t="shared" si="11"/>
+        <v>0.32019117591767426</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5">
       <c r="A119" s="2"/>
       <c r="B119" t="s">
         <v>386</v>
@@ -59577,8 +60011,12 @@
       <c r="D119">
         <v>178195622</v>
       </c>
-    </row>
-    <row r="120" spans="1:4">
+      <c r="E119" s="7">
+        <f t="shared" si="11"/>
+        <v>0.49996510517332748</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5">
       <c r="A120" s="2"/>
       <c r="B120" t="s">
         <v>387</v>
@@ -59589,11 +60027,15 @@
       <c r="D120">
         <v>632719623</v>
       </c>
-    </row>
-    <row r="121" spans="1:4">
+      <c r="E120" s="7">
+        <f t="shared" si="11"/>
+        <v>1.503510684002916</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:4">
+    <row r="122" spans="1:5">
       <c r="A122" s="2" t="s">
         <v>403</v>
       </c>
@@ -59606,8 +60048,12 @@
       <c r="D122">
         <v>71049210305</v>
       </c>
-    </row>
-    <row r="123" spans="1:4">
+      <c r="E122" s="7">
+        <f>+(D122-C122)/C122</f>
+        <v>0.31206990826843156</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5">
       <c r="A123" s="2"/>
       <c r="B123" t="s">
         <v>380</v>
@@ -59618,8 +60064,12 @@
       <c r="D123">
         <v>68147358853</v>
       </c>
-    </row>
-    <row r="124" spans="1:4">
+      <c r="E123" s="7">
+        <f t="shared" ref="E123:E130" si="12">+(D123-C123)/C123</f>
+        <v>0.26548180758875656</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5">
       <c r="A124" s="2"/>
       <c r="B124" t="s">
         <v>381</v>
@@ -59630,8 +60080,12 @@
       <c r="D124">
         <v>42184376230</v>
       </c>
-    </row>
-    <row r="125" spans="1:4">
+      <c r="E124" s="7">
+        <f t="shared" si="12"/>
+        <v>0.44181695785301378</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5">
       <c r="A125" s="2"/>
       <c r="B125" t="s">
         <v>382</v>
@@ -59642,8 +60096,12 @@
       <c r="D125">
         <v>25962982623</v>
       </c>
-    </row>
-    <row r="126" spans="1:4">
+      <c r="E125" s="7">
+        <f t="shared" si="12"/>
+        <v>5.5700600230210798E-2</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5">
       <c r="A126" s="2"/>
       <c r="B126" t="s">
         <v>383</v>
@@ -59654,8 +60112,12 @@
       <c r="D126">
         <v>1355399711</v>
       </c>
-    </row>
-    <row r="127" spans="1:4">
+      <c r="E126" s="7">
+        <f t="shared" si="12"/>
+        <v>0.96474155148631413</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5">
       <c r="A127" s="2"/>
       <c r="B127" t="s">
         <v>384</v>
@@ -59666,8 +60128,12 @@
       <c r="D127">
         <v>147286894</v>
       </c>
-    </row>
-    <row r="128" spans="1:4">
+      <c r="E127" s="7">
+        <f t="shared" si="12"/>
+        <v>0.38721740688741357</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
       <c r="A128" s="2"/>
       <c r="B128" t="s">
         <v>385</v>
@@ -59678,8 +60144,12 @@
       <c r="D128">
         <v>345013370</v>
       </c>
-    </row>
-    <row r="129" spans="1:4">
+      <c r="E128" s="7">
+        <f t="shared" si="12"/>
+        <v>0.46228912245106712</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5">
       <c r="A129" s="2"/>
       <c r="B129" t="s">
         <v>386</v>
@@ -59690,8 +60160,12 @@
       <c r="D129">
         <v>174723163</v>
       </c>
-    </row>
-    <row r="130" spans="1:4">
+      <c r="E129" s="7">
+        <f t="shared" si="12"/>
+        <v>0.43733936550842178</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5">
       <c r="A130" s="2"/>
       <c r="B130" t="s">
         <v>387</v>
@@ -59702,11 +60176,15 @@
       <c r="D130">
         <v>688376284</v>
       </c>
-    </row>
-    <row r="131" spans="1:4">
+      <c r="E130" s="7">
+        <f t="shared" si="12"/>
+        <v>2.0434011605882296</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5">
       <c r="A131" s="2"/>
     </row>
-    <row r="132" spans="1:4">
+    <row r="132" spans="1:5">
       <c r="A132" s="2" t="s">
         <v>33</v>
       </c>
@@ -59719,8 +60197,12 @@
       <c r="D132">
         <v>69513385821</v>
       </c>
-    </row>
-    <row r="133" spans="1:4">
+      <c r="E132" s="7">
+        <f>+(D132-C132)/C132</f>
+        <v>0.28724111345754083</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5">
       <c r="A133" s="2"/>
       <c r="B133" t="s">
         <v>380</v>
@@ -59731,8 +60213,12 @@
       <c r="D133">
         <v>69431872627</v>
       </c>
-    </row>
-    <row r="134" spans="1:4">
+      <c r="E133" s="7">
+        <f t="shared" ref="E133:E140" si="13">+(D133-C133)/C133</f>
+        <v>0.36508996835157809</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5">
       <c r="A134" s="2"/>
       <c r="B134" t="s">
         <v>381</v>
@@ -59743,8 +60229,12 @@
       <c r="D134">
         <v>41738895626</v>
       </c>
-    </row>
-    <row r="135" spans="1:4">
+      <c r="E134" s="7">
+        <f t="shared" si="13"/>
+        <v>0.42979682075904779</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5">
       <c r="A135" s="2"/>
       <c r="B135" t="s">
         <v>382</v>
@@ -59755,8 +60245,12 @@
       <c r="D135">
         <v>27692977001</v>
       </c>
-    </row>
-    <row r="136" spans="1:4">
+      <c r="E135" s="7">
+        <f t="shared" si="13"/>
+        <v>0.27792299973917062</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5">
       <c r="A136" s="2"/>
       <c r="B136" t="s">
         <v>383</v>
@@ -59767,8 +60261,12 @@
       <c r="D136">
         <v>1333703377</v>
       </c>
-    </row>
-    <row r="137" spans="1:4">
+      <c r="E136" s="7">
+        <f t="shared" si="13"/>
+        <v>0.91952006420509935</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5">
       <c r="A137" s="2"/>
       <c r="B137" t="s">
         <v>384</v>
@@ -59779,8 +60277,12 @@
       <c r="D137">
         <v>140466832</v>
       </c>
-    </row>
-    <row r="138" spans="1:4">
+      <c r="E137" s="7">
+        <f t="shared" si="13"/>
+        <v>0.4144456899764189</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5">
       <c r="A138" s="2"/>
       <c r="B138" t="s">
         <v>385</v>
@@ -59791,8 +60293,12 @@
       <c r="D138">
         <v>301512528</v>
       </c>
-    </row>
-    <row r="139" spans="1:4">
+      <c r="E138" s="7">
+        <f t="shared" si="13"/>
+        <v>0.27863075845072388</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5">
       <c r="A139" s="2"/>
       <c r="B139" t="s">
         <v>386</v>
@@ -59803,8 +60309,12 @@
       <c r="D139">
         <v>196974648</v>
       </c>
-    </row>
-    <row r="140" spans="1:4">
+      <c r="E139" s="7">
+        <f t="shared" si="13"/>
+        <v>0.52152737010744554</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5">
       <c r="A140" s="2"/>
       <c r="B140" t="s">
         <v>387</v>
@@ -59815,11 +60325,15 @@
       <c r="D140">
         <v>694749369</v>
       </c>
-    </row>
-    <row r="141" spans="1:4">
+      <c r="E140" s="7">
+        <f t="shared" si="13"/>
+        <v>2.0175702492729419</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:4">
+    <row r="142" spans="1:5">
       <c r="A142" s="2" t="s">
         <v>404</v>
       </c>
@@ -59832,8 +60346,12 @@
       <c r="D142">
         <v>44776666110</v>
       </c>
-    </row>
-    <row r="143" spans="1:4">
+      <c r="E142" s="7">
+        <f>+(D142-C142)/C142</f>
+        <v>-0.29744917323041148</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5">
       <c r="A143" s="2"/>
       <c r="B143" t="s">
         <v>380</v>
@@ -59844,8 +60362,12 @@
       <c r="D143">
         <v>45103734069</v>
       </c>
-    </row>
-    <row r="144" spans="1:4">
+      <c r="E143" s="7">
+        <f t="shared" ref="E143:E150" si="14">+(D143-C143)/C143</f>
+        <v>-0.28140148161793294</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5">
       <c r="A144" s="2"/>
       <c r="B144" t="s">
         <v>381</v>
@@ -59856,8 +60378,12 @@
       <c r="D144">
         <v>2890157713</v>
       </c>
-    </row>
-    <row r="145" spans="1:4">
+      <c r="E144" s="7">
+        <f t="shared" si="14"/>
+        <v>-0.79853569320817097</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
       <c r="A145" s="2"/>
       <c r="B145" t="s">
         <v>382</v>
@@ -59868,8 +60394,12 @@
       <c r="D145">
         <v>42213576356</v>
       </c>
-    </row>
-    <row r="146" spans="1:4">
+      <c r="E145" s="7">
+        <f t="shared" si="14"/>
+        <v>-0.12818782359772266</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
       <c r="A146" s="2"/>
       <c r="B146" t="s">
         <v>383</v>
@@ -59880,8 +60410,12 @@
       <c r="D146">
         <v>1634002706</v>
       </c>
-    </row>
-    <row r="147" spans="1:4">
+      <c r="E146" s="7">
+        <f t="shared" si="14"/>
+        <v>-0.36637317522742097</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
       <c r="A147" s="2"/>
       <c r="B147" t="s">
         <v>384</v>
@@ -59892,8 +60426,12 @@
       <c r="D147">
         <v>907772872</v>
       </c>
-    </row>
-    <row r="148" spans="1:4">
+      <c r="E147" s="7">
+        <f t="shared" si="14"/>
+        <v>-9.4903595817579067E-2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
       <c r="A148" s="2"/>
       <c r="B148" t="s">
         <v>385</v>
@@ -59904,8 +60442,12 @@
       <c r="D148">
         <v>425490701</v>
       </c>
-    </row>
-    <row r="149" spans="1:4">
+      <c r="E148" s="7">
+        <f t="shared" si="14"/>
+        <v>-2.7928816305622058E-2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
       <c r="A149" s="2"/>
       <c r="B149" t="s">
         <v>386</v>
@@ -59916,8 +60458,12 @@
       <c r="D149">
         <v>154047385</v>
       </c>
-    </row>
-    <row r="150" spans="1:4">
+      <c r="E149" s="7">
+        <f t="shared" si="14"/>
+        <v>-0.39593256157418233</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
       <c r="A150" s="2"/>
       <c r="B150" t="s">
         <v>387</v>
@@ -59928,32 +60474,36 @@
       <c r="D150">
         <v>146691748</v>
       </c>
-    </row>
-    <row r="152" spans="1:4">
+      <c r="E150" s="7">
+        <f t="shared" si="14"/>
+        <v>-0.8338936937743251</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5">
       <c r="A152" s="2"/>
     </row>
-    <row r="153" spans="1:4">
+    <row r="153" spans="1:5">
       <c r="A153" s="2"/>
     </row>
-    <row r="154" spans="1:4">
+    <row r="154" spans="1:5">
       <c r="A154" s="2"/>
     </row>
-    <row r="155" spans="1:4">
+    <row r="155" spans="1:5">
       <c r="A155" s="2"/>
     </row>
-    <row r="156" spans="1:4">
+    <row r="156" spans="1:5">
       <c r="A156" s="2"/>
     </row>
-    <row r="157" spans="1:4">
+    <row r="157" spans="1:5">
       <c r="A157" s="2"/>
     </row>
-    <row r="158" spans="1:4">
+    <row r="158" spans="1:5">
       <c r="A158" s="2"/>
     </row>
-    <row r="159" spans="1:4">
+    <row r="159" spans="1:5">
       <c r="A159" s="2"/>
     </row>
-    <row r="160" spans="1:4">
+    <row r="160" spans="1:5">
       <c r="A160" s="2"/>
     </row>
     <row r="161" spans="1:1">
@@ -60078,7 +60628,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
improvement hw counters excel special case
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11555" uniqueCount="407">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11557" uniqueCount="408">
   <si>
     <t>----------------------</t>
   </si>
@@ -1263,6 +1263,9 @@
   <si>
     <t>Improvement</t>
   </si>
+  <si>
+    <t>Comparison</t>
+  </si>
 </sst>
 </file>
 
@@ -1333,7 +1336,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="326">
+  <cellStyleXfs count="342">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1660,6 +1663,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1673,7 +1692,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="313" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="326">
+  <cellStyles count="342">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1836,6 +1855,14 @@
     <cellStyle name="Followed Hyperlink" xfId="321" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="323" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="325" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="327" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="329" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="331" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="333" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="335" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="337" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="339" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="341" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1998,6 +2025,14 @@
     <cellStyle name="Hyperlink" xfId="320" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="322" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="324" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="326" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="328" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="330" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="332" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="334" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="336" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="338" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="340" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="313" builtinId="5"/>
   </cellStyles>
@@ -4156,6 +4191,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -4192,6 +4228,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4205,6 +4242,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4505,6 +4543,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -4541,6 +4580,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4554,6 +4594,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4899,6 +4940,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
@@ -4935,6 +4977,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
@@ -4948,6 +4991,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -50745,8 +50789,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView topLeftCell="B35" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58322,10 +58366,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H200"/>
+  <dimension ref="A1:I200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="I132" sqref="I132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -58335,6 +58379,7 @@
     <col min="3" max="3" width="39.6640625" customWidth="1"/>
     <col min="4" max="4" width="39.83203125" customWidth="1"/>
     <col min="5" max="5" width="25.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -60149,7 +60194,7 @@
         <v>0.46228912245106712</v>
       </c>
     </row>
-    <row r="129" spans="1:5">
+    <row r="129" spans="1:9">
       <c r="A129" s="2"/>
       <c r="B129" t="s">
         <v>386</v>
@@ -60165,7 +60210,7 @@
         <v>0.43733936550842178</v>
       </c>
     </row>
-    <row r="130" spans="1:5">
+    <row r="130" spans="1:9">
       <c r="A130" s="2"/>
       <c r="B130" t="s">
         <v>387</v>
@@ -60181,10 +60226,16 @@
         <v>2.0434011605882296</v>
       </c>
     </row>
-    <row r="131" spans="1:5">
+    <row r="131" spans="1:9">
       <c r="A131" s="2"/>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="G131" t="s">
+        <v>28</v>
+      </c>
+      <c r="I131" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9">
       <c r="A132" s="2" t="s">
         <v>33</v>
       </c>
@@ -60201,8 +60252,15 @@
         <f>+(D132-C132)/C132</f>
         <v>0.28724111345754083</v>
       </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="G132" s="7">
+        <v>0.44919484442667712</v>
+      </c>
+      <c r="I132" s="1">
+        <f>+G132-E132</f>
+        <v>0.16195373096913629</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9">
       <c r="A133" s="2"/>
       <c r="B133" t="s">
         <v>380</v>
@@ -60217,8 +60275,15 @@
         <f t="shared" ref="E133:E140" si="13">+(D133-C133)/C133</f>
         <v>0.36508996835157809</v>
       </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="G133" s="7">
+        <v>0.44977063674646239</v>
+      </c>
+      <c r="I133" s="1">
+        <f t="shared" ref="I133:I140" si="14">+G133-E133</f>
+        <v>8.4680668394884306E-2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9">
       <c r="A134" s="2"/>
       <c r="B134" t="s">
         <v>381</v>
@@ -60233,8 +60298,15 @@
         <f t="shared" si="13"/>
         <v>0.42979682075904779</v>
       </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="G134" s="7">
+        <v>0.62460911677382269</v>
+      </c>
+      <c r="I134" s="1">
+        <f t="shared" si="14"/>
+        <v>0.1948122960147749</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9">
       <c r="A135" s="2"/>
       <c r="B135" t="s">
         <v>382</v>
@@ -60249,8 +60321,15 @@
         <f t="shared" si="13"/>
         <v>0.27792299973917062</v>
       </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="G135" s="7">
+        <v>0.23119960065998979</v>
+      </c>
+      <c r="I135" s="1">
+        <f t="shared" si="14"/>
+        <v>-4.6723399079180827E-2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9">
       <c r="A136" s="2"/>
       <c r="B136" t="s">
         <v>383</v>
@@ -60265,8 +60344,15 @@
         <f t="shared" si="13"/>
         <v>0.91952006420509935</v>
       </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="G136" s="7">
+        <v>0.85200576053552191</v>
+      </c>
+      <c r="I136" s="1">
+        <f t="shared" si="14"/>
+        <v>-6.7514303669577447E-2</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9">
       <c r="A137" s="2"/>
       <c r="B137" t="s">
         <v>384</v>
@@ -60281,8 +60367,15 @@
         <f t="shared" si="13"/>
         <v>0.4144456899764189</v>
       </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="G137" s="7">
+        <v>0.69917789027128618</v>
+      </c>
+      <c r="I137" s="1">
+        <f t="shared" si="14"/>
+        <v>0.28473220029486729</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9">
       <c r="A138" s="2"/>
       <c r="B138" t="s">
         <v>385</v>
@@ -60297,8 +60390,15 @@
         <f t="shared" si="13"/>
         <v>0.27863075845072388</v>
       </c>
-    </row>
-    <row r="139" spans="1:5">
+      <c r="G138" s="7">
+        <v>0.44683704766766247</v>
+      </c>
+      <c r="I138" s="1">
+        <f t="shared" si="14"/>
+        <v>0.16820628921693859</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9">
       <c r="A139" s="2"/>
       <c r="B139" t="s">
         <v>386</v>
@@ -60313,8 +60413,15 @@
         <f t="shared" si="13"/>
         <v>0.52152737010744554</v>
       </c>
-    </row>
-    <row r="140" spans="1:5">
+      <c r="G139" s="7">
+        <v>-8.0898106135577057E-3</v>
+      </c>
+      <c r="I139" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.52961718072100328</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9">
       <c r="A140" s="2"/>
       <c r="B140" t="s">
         <v>387</v>
@@ -60329,11 +60436,18 @@
         <f t="shared" si="13"/>
         <v>2.0175702492729419</v>
       </c>
-    </row>
-    <row r="141" spans="1:5">
+      <c r="G140" s="7">
+        <v>1.7249229019702748</v>
+      </c>
+      <c r="I140" s="1">
+        <f t="shared" si="14"/>
+        <v>-0.29264734730266717</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:5">
+    <row r="142" spans="1:9">
       <c r="A142" s="2" t="s">
         <v>404</v>
       </c>
@@ -60351,7 +60465,7 @@
         <v>-0.29744917323041148</v>
       </c>
     </row>
-    <row r="143" spans="1:5">
+    <row r="143" spans="1:9">
       <c r="A143" s="2"/>
       <c r="B143" t="s">
         <v>380</v>
@@ -60363,11 +60477,11 @@
         <v>45103734069</v>
       </c>
       <c r="E143" s="7">
-        <f t="shared" ref="E143:E150" si="14">+(D143-C143)/C143</f>
+        <f t="shared" ref="E143:E150" si="15">+(D143-C143)/C143</f>
         <v>-0.28140148161793294</v>
       </c>
     </row>
-    <row r="144" spans="1:5">
+    <row r="144" spans="1:9">
       <c r="A144" s="2"/>
       <c r="B144" t="s">
         <v>381</v>
@@ -60379,7 +60493,7 @@
         <v>2890157713</v>
       </c>
       <c r="E144" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.79853569320817097</v>
       </c>
     </row>
@@ -60395,7 +60509,7 @@
         <v>42213576356</v>
       </c>
       <c r="E145" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.12818782359772266</v>
       </c>
     </row>
@@ -60411,7 +60525,7 @@
         <v>1634002706</v>
       </c>
       <c r="E146" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.36637317522742097</v>
       </c>
     </row>
@@ -60427,7 +60541,7 @@
         <v>907772872</v>
       </c>
       <c r="E147" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-9.4903595817579067E-2</v>
       </c>
     </row>
@@ -60443,7 +60557,7 @@
         <v>425490701</v>
       </c>
       <c r="E148" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-2.7928816305622058E-2</v>
       </c>
     </row>
@@ -60459,7 +60573,7 @@
         <v>154047385</v>
       </c>
       <c r="E149" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.39593256157418233</v>
       </c>
     </row>
@@ -60475,7 +60589,7 @@
         <v>146691748</v>
       </c>
       <c r="E150" s="7">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.8338936937743251</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New graph and text.
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27520" windowHeight="18080" tabRatio="915" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14580" tabRatio="915" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="experiment_timings.txt" sheetId="1" r:id="rId1"/>
@@ -1349,6 +1349,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1408,7 +1409,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="794">
+  <cellStyleXfs count="796">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2203,6 +2204,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2220,7 +2223,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="794">
+  <cellStyles count="796">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2617,6 +2620,7 @@
     <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="793" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="795" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3013,6 +3017,7 @@
     <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="792" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="794" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="313" builtinId="5"/>
   </cellStyles>
@@ -3328,11 +3333,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2145648968"/>
-        <c:axId val="-2145642040"/>
+        <c:axId val="2068212248"/>
+        <c:axId val="2067319080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2145648968"/>
+        <c:axId val="2068212248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3367,7 +3372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145642040"/>
+        <c:crossAx val="2067319080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3375,7 +3380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2145642040"/>
+        <c:axId val="2067319080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3404,7 +3409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2145648968"/>
+        <c:crossAx val="2068212248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3728,7 +3733,6 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -4124,11 +4128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2063563240"/>
-        <c:axId val="2063569112"/>
+        <c:axId val="-2125046456"/>
+        <c:axId val="-2125040568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2063563240"/>
+        <c:axId val="-2125046456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4157,13 +4161,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063569112"/>
+        <c:crossAx val="-2125040568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4171,7 +4174,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2063569112"/>
+        <c:axId val="-2125040568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4194,21 +4197,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063563240"/>
+        <c:crossAx val="-2125046456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -4913,11 +4914,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144689032"/>
-        <c:axId val="-2144683112"/>
+        <c:axId val="-2124982744"/>
+        <c:axId val="-2124976856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144689032"/>
+        <c:axId val="-2124982744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4946,13 +4947,12 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144683112"/>
+        <c:crossAx val="-2124976856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4960,7 +4960,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144683112"/>
+        <c:axId val="-2124976856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4983,21 +4983,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144689032"/>
+        <c:crossAx val="-2124982744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5026,7 +5024,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -6149,20 +6147,92 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144585928"/>
-        <c:axId val="-2144583016"/>
+        <c:axId val="-2124880392"/>
+        <c:axId val="-2124877480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144585928"/>
+        <c:axId val="-2124880392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+              <a:p>
+                <a:pPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US" sz="1000"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144583016"/>
+        <c:crossAx val="-2124877480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6170,7 +6240,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144583016"/>
+        <c:axId val="-2124877480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6200,7 +6270,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144585928"/>
+        <c:crossAx val="-2124880392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6240,6 +6310,1242 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$147</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DCACHE_MISS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$147:$W$147</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.6823446998E10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5000788104E10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4956518295E10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.3444008334E10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.1589134651E10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.4973262446E10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1816150065E10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3408381302E10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.3967871539E10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.183666574E10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.0294981125E10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3434025259E10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.4150476173E10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.4001837802E10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.3734415225E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$148</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_L2L3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$148:$W$148</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>7.9778731885E10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1806406138E10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.179879199E10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2815077778E10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0976624288E10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.0370745035E10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.1471532542E10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3581592326E10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5.2152276424E10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.584568852E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4598990298E10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.3156067137E10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.3850919424E10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5.0862488361E10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6.2766249742E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$149</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_L2L3_CONFLICT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$149:$W$149</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>4.4651870248E10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.35563099E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.94810637E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8849987576E10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.173417022E9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.9769420401E10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.779538349E10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.9006613026E10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8974838242E10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.83909679E8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.8733255021E10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.8516765508E10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.9257788931E10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.9192186624E10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.4345755628E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$150</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_L2L3_NO_CONFLICT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$150:$W$150</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>3.5126861637E10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0870843039E10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1003981353E10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3965090202E10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.803207266E9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.0601324634E10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3676149052E10</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.45749793E10</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.3177438182E10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.300659173E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.5865735277E10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.4639301629E10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.4593130493E10</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.1670301737E10</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.8420494114E10</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$151</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_L3MISS</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$151:$W$151</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>9.69530311E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.378869371E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.318334859E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.42250849E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5490409E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.92602746E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.08653588E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.35707377E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.23115409E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.146714871E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9.60968156E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.0700675E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.8986158E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.94810855E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.578809233E9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$152</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_LMEM</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$152:$W$152</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>1.96911623E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.53621706E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.523429304E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.03676497E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.05692432E8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.82917002E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.8677218E7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.8194096E7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.9313385E7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.794260352E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.65400964E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.2057738E7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.06174341E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9.9308749E7</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.002957108E9</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$153</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_L21_L31</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$153:$W$153</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.76669105E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.81261912E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.78801748E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.46517287E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6060227E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.87337539E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.38927533E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.33380808E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.33763466E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.14663728E8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.76692789E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.43416224E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.35940598E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.35808912E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.37715579E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$154</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_REMOTE</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$154:$W$154</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.37667898E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.07371106E8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.16962688E8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.34117249E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1866357E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.26997597E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.22949716E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.33793482E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.33051446E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.04098019E8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.39934256E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.18799845E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.21560132E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.29458498E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.55016866E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$H$155</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>_PM_CMPLU_STALL_DMISS_DISTANT</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$146:$W$146</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$I$155:$W$155</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.58281685E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.454019293E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.399141119E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.57939816E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1285074E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5350608E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.48099121E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.70338991E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.56987112E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.033692772E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.78940147E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.52732943E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.26186509E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.30234696E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8311968E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2125564936"/>
+        <c:axId val="2079890264"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2125564936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1000" b="1" i="0" baseline="0">
+                    <a:effectLst/>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>OpenMP Affinity (OMP_PROC_BIND, OMP_PLACES)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1000">
+                  <a:effectLst/>
+                  <a:latin typeface="+mn-lt"/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2079890264"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2079890264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Stall Cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2125564936"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
@@ -6540,11 +7846,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144536360"/>
-        <c:axId val="-2144530264"/>
+        <c:axId val="-2124828072"/>
+        <c:axId val="-2124821976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144536360"/>
+        <c:axId val="-2124828072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6597,7 +7903,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144530264"/>
+        <c:crossAx val="-2124821976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6605,7 +7911,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144530264"/>
+        <c:axId val="-2124821976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6635,7 +7941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144536360"/>
+        <c:crossAx val="-2124828072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6842,11 +8148,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144828488"/>
-        <c:axId val="-2144822920"/>
+        <c:axId val="2085993000"/>
+        <c:axId val="2066955240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144828488"/>
+        <c:axId val="2085993000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6873,7 +8179,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144822920"/>
+        <c:crossAx val="2066955240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6881,7 +8187,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144822920"/>
+        <c:axId val="2066955240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6915,7 +8221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144828488"/>
+        <c:crossAx val="2085993000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7103,11 +8409,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146592168"/>
-        <c:axId val="-2146586632"/>
+        <c:axId val="2124235336"/>
+        <c:axId val="2124240872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146592168"/>
+        <c:axId val="2124235336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7134,7 +8440,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146586632"/>
+        <c:crossAx val="2124240872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7142,7 +8448,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146586632"/>
+        <c:axId val="2124240872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7171,7 +8477,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146592168"/>
+        <c:crossAx val="2124235336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7468,11 +8774,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146525848"/>
-        <c:axId val="-2146520216"/>
+        <c:axId val="-2125213960"/>
+        <c:axId val="-2125208280"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146525848"/>
+        <c:axId val="-2125213960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7498,12 +8804,13 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146520216"/>
+        <c:crossAx val="-2125208280"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7511,7 +8818,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146520216"/>
+        <c:axId val="-2125208280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7539,19 +8846,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146525848"/>
+        <c:crossAx val="-2125213960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -7751,11 +9060,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146489176"/>
-        <c:axId val="-2146483608"/>
+        <c:axId val="-2125176888"/>
+        <c:axId val="-2125171304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146489176"/>
+        <c:axId val="-2125176888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7782,7 +9091,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146483608"/>
+        <c:crossAx val="-2125171304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7790,7 +9099,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2146483608"/>
+        <c:axId val="-2125171304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7819,7 +9128,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146489176"/>
+        <c:crossAx val="-2125176888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8012,11 +9321,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2146454104"/>
-        <c:axId val="-2147453160"/>
+        <c:axId val="-2125142264"/>
+        <c:axId val="-2125136712"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2146454104"/>
+        <c:axId val="-2125142264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8043,7 +9352,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2147453160"/>
+        <c:crossAx val="-2125136712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8051,7 +9360,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2147453160"/>
+        <c:axId val="-2125136712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8080,7 +9389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2146454104"/>
+        <c:crossAx val="-2125142264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8377,11 +9686,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144763912"/>
-        <c:axId val="-2144758344"/>
+        <c:axId val="2085955336"/>
+        <c:axId val="2068222792"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144763912"/>
+        <c:axId val="2085955336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8408,7 +9717,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144758344"/>
+        <c:crossAx val="2068222792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8416,7 +9725,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144758344"/>
+        <c:axId val="2068222792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8445,7 +9754,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144763912"/>
+        <c:crossAx val="2085955336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8726,11 +10035,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-2144726024"/>
-        <c:axId val="-2144720456"/>
+        <c:axId val="2086165768"/>
+        <c:axId val="2085749832"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2144726024"/>
+        <c:axId val="2086165768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8757,7 +10066,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144720456"/>
+        <c:crossAx val="2085749832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8765,7 +10074,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2144720456"/>
+        <c:axId val="2085749832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8794,7 +10103,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2144726024"/>
+        <c:crossAx val="2086165768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9109,11 +10418,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2063484792"/>
-        <c:axId val="2063490936"/>
+        <c:axId val="-2125126136"/>
+        <c:axId val="-2125120072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2063484792"/>
+        <c:axId val="-2125126136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9169,7 +10478,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063490936"/>
+        <c:crossAx val="-2125120072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9177,7 +10486,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2063490936"/>
+        <c:axId val="-2125120072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9206,7 +10515,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2063484792"/>
+        <c:crossAx val="-2125126136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9604,6 +10913,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>165100</xdr:colOff>
+      <xdr:row>160</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -15964,7 +17303,7 @@
   <dimension ref="J1:M86"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -64835,8 +66174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J120" workbookViewId="0">
-      <selection activeCell="L130" sqref="L130"/>
+    <sheetView tabSelected="1" topLeftCell="R127" workbookViewId="0">
+      <selection activeCell="H146" sqref="H146:W155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>

<commit_message>
All corrections suggested by Oscar and reviewers.
</commit_message>
<xml_diff>
--- a/Data/graphs_experiments.xlsx
+++ b/Data/graphs_experiments.xlsx
@@ -1415,7 +1415,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="874">
+  <cellStyleXfs count="876">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2290,6 +2290,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2307,7 +2309,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="874">
+  <cellStyles count="876">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2744,6 +2746,7 @@
     <cellStyle name="Followed Hyperlink" xfId="869" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="871" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="873" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="875" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3180,6 +3183,7 @@
     <cellStyle name="Hyperlink" xfId="868" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="870" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="872" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="874" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="313" builtinId="5"/>
   </cellStyles>
@@ -8469,6 +8473,336 @@
 </file>
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$J$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Good data locality</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$73:$I$87</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$J$73:$J$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>2.58281685E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.454019293E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.399141119E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.57939816E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1285074E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.5350608E7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.48099121E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.70338991E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.56987112E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.033692772E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.78940147E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.52732943E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.26186509E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.30234696E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.8311968E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>HW_20_Final!$K$72</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bad data locality</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>HW_20_Final!$I$73:$I$87</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>(false,threads)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>(true,threads)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>(close,threads)</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>(spread, threads)</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>(master,threads)</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>(false,cores)</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>(true,cores)</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>(close,cores)</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>(spread, cores)</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>(master,cores)</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>(false,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>(true,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>(close,sockets)</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>(spread, sockets)</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>(master,sockets)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>HW_20_Final!$K$73:$K$87</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>6.41037327E8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.261190085E9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.201384463E9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.22039624E8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4694927E7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.11501178E8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.46114763E8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.61752057E8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.00270067E8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.126454532E9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.30094631E8</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>6.32719623E8</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.88376284E8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.94749369E8</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.46691748E8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2125354424"/>
+        <c:axId val="-2128678920"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2125354424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2128678920"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2128678920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2125354424"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -11949,6 +12283,36 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1443566</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>897466</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -67180,8 +67544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W200"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86:K86"/>
+    <sheetView tabSelected="1" topLeftCell="D86" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="I72" sqref="I72:K87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -68797,6 +69161,12 @@
       <c r="I87" t="s">
         <v>404</v>
       </c>
+      <c r="J87">
+        <v>883119680</v>
+      </c>
+      <c r="K87">
+        <v>146691748</v>
+      </c>
     </row>
     <row r="88" spans="1:23">
       <c r="B88" t="s">

</xml_diff>